<commit_message>
Deleted lossess_all output, as it's in the pdf so a duplicate
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubey\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA422312-3E66-4A0E-8BF7-2E8FB6EFA027}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B5BE7B-776E-418D-A0DA-A65AD124EC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4524" yWindow="864" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -42,23 +42,58 @@
     <t>recognizeStokes4.py</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>recognizeStokes.py</t>
-  </si>
-  <si>
-    <t>Running 5 models each on linux, 4=&gt; means CNN4</t>
-  </si>
-  <si>
-    <t>Running 5 models each on linux, =&gt; means CNN1</t>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>recognizeStokes2.py</t>
+  </si>
+  <si>
+    <t>recognizeStokes3.py</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Cont.?</t>
+  </si>
+  <si>
+    <t>Job id</t>
+  </si>
+  <si>
+    <t>Running?</t>
+  </si>
+  <si>
+    <t>Rerunning 3 more, 2 was not good</t>
+  </si>
+  <si>
+    <t>recognizeStokes1.py</t>
+  </si>
+  <si>
+    <t>3_1; 3_2 are not good. Running 3 more</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2_1; 2_2 =&gt; are good. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Running 3 more</t>
+    </r>
+  </si>
+  <si>
+    <t>The first run not finished yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +105,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,9 +143,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -380,53 +435,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C15:D22"/>
+  <dimension ref="B3:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="69.5546875" customWidth="1"/>
+    <col min="4" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="59.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="1" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>809906</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>809914</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>809915</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>809918</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>809804</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added Keras data augmentation by rotation. Runs ok. Will put to Linux.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B5BE7B-776E-418D-A0DA-A65AD124EC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4E3F72-4673-4934-AAAE-205F1988A9FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4524" yWindow="864" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1596" yWindow="5712" windowWidth="19536" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>The first run not finished yet</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Not much improvement</t>
   </si>
 </sst>
 </file>
@@ -435,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:G9"/>
+  <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,9 +455,10 @@
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="7" width="59.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -467,8 +477,11 @@
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>809906</v>
       </c>
@@ -482,13 +495,16 @@
         <v>8</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>809914</v>
       </c>
@@ -506,7 +522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>809915</v>
       </c>
@@ -524,7 +540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>809918</v>
       </c>
@@ -542,7 +558,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>809804</v>
       </c>

</xml_diff>

<commit_message>
Changed CNN3, and removes some Keras warning e.g. fit_fenerator to 'fit'
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4E3F72-4673-4934-AAAE-205F1988A9FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDCE030-EAD5-4C5E-8CFB-4FADA65AEC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1596" yWindow="5712" windowWidth="19536" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
   <si>
-    <t>Name in Linux</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
@@ -63,13 +60,7 @@
     <t>Running?</t>
   </si>
   <si>
-    <t>Rerunning 3 more, 2 was not good</t>
-  </si>
-  <si>
     <t>recognizeStokes1.py</t>
-  </si>
-  <si>
-    <t>3_1; 3_2 are not good. Running 3 more</t>
   </si>
   <si>
     <r>
@@ -86,16 +77,76 @@
     </r>
   </si>
   <si>
-    <t>The first run not finished yet</t>
-  </si>
-  <si>
-    <t>Finished</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
     <t>Not much improvement</t>
+  </si>
+  <si>
+    <t>my laptop</t>
+  </si>
+  <si>
+    <t>recognizeStokes.py</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>4_1 not good</t>
+  </si>
+  <si>
+    <t>Keras augmentation rotation</t>
+  </si>
+  <si>
+    <t>"selu", receptive field = (7,7) ten decreease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_1; 3_2; 3_1; 3_1; 3_2 are not good. </t>
+  </si>
+  <si>
+    <t>Why this is always bad?</t>
+  </si>
+  <si>
+    <t>4_1 is not good, 4_2 not good enough</t>
+  </si>
+  <si>
+    <t>Subcases</t>
+  </si>
+  <si>
+    <t>case1.py</t>
+  </si>
+  <si>
+    <t>case2.py</t>
+  </si>
+  <si>
+    <t>10,11</t>
+  </si>
+  <si>
+    <t>3 were not good</t>
+  </si>
+  <si>
+    <t>Rerunning 2 more</t>
+  </si>
+  <si>
+    <t>Saved as</t>
+  </si>
+  <si>
+    <t>model_cnn2_2.h5py / model_cnn2_1.h5py</t>
+  </si>
+  <si>
+    <t>case3.py</t>
+  </si>
+  <si>
+    <t>12,13</t>
+  </si>
+  <si>
+    <t>case4.py</t>
+  </si>
+  <si>
+    <t>3new</t>
+  </si>
+  <si>
+    <t>CNN3 updated exactly as in website, but 'LeakyRELU'</t>
   </si>
 </sst>
 </file>
@@ -132,12 +183,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,16 +209,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -444,139 +505,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:H9"/>
+  <dimension ref="B3:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="59.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="59.44140625" customWidth="1"/>
+    <col min="9" max="9" width="31.109375" customWidth="1"/>
+    <col min="10" max="10" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="H3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>809914</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>809915</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>809918</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>809804</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>809906</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="G9" s="3"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="G10" s="3"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>809914</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>810164</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>809915</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>810163</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>809918</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>809804</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2">
-        <v>4</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>810174</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>810175</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="J12:Q12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified CNN architecture and run.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDCE030-EAD5-4C5E-8CFB-4FADA65AEC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E59DC77-06FE-4FAD-AA4E-B443E3F5E20A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -63,20 +63,6 @@
     <t>recognizeStokes1.py</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">2_1; 2_2 =&gt; are good. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Running 3 more</t>
-    </r>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
@@ -92,21 +78,12 @@
     <t>Name</t>
   </si>
   <si>
-    <t>4_1 not good</t>
-  </si>
-  <si>
     <t>Keras augmentation rotation</t>
   </si>
   <si>
     <t>"selu", receptive field = (7,7) ten decreease</t>
   </si>
   <si>
-    <t xml:space="preserve">3_1; 3_2; 3_1; 3_1; 3_2 are not good. </t>
-  </si>
-  <si>
-    <t>Why this is always bad?</t>
-  </si>
-  <si>
     <t>4_1 is not good, 4_2 not good enough</t>
   </si>
   <si>
@@ -122,18 +99,9 @@
     <t>10,11</t>
   </si>
   <si>
-    <t>3 were not good</t>
-  </si>
-  <si>
-    <t>Rerunning 2 more</t>
-  </si>
-  <si>
     <t>Saved as</t>
   </si>
   <si>
-    <t>model_cnn2_2.h5py / model_cnn2_1.h5py</t>
-  </si>
-  <si>
     <t>case3.py</t>
   </si>
   <si>
@@ -143,10 +111,133 @@
     <t>case4.py</t>
   </si>
   <si>
-    <t>3new</t>
-  </si>
-  <si>
     <t>CNN3 updated exactly as in website, but 'LeakyRELU'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_1; 3_2; 3_1; 3_1; 3_2 are not good. Why this is always bad? </t>
+  </si>
+  <si>
+    <t>selu</t>
+  </si>
+  <si>
+    <t>Activation</t>
+  </si>
+  <si>
+    <t>leakyRELU</t>
+  </si>
+  <si>
+    <t>very bad</t>
+  </si>
+  <si>
+    <t>"elu"</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1_3 is fairly good, but not best. Others are awful. </t>
+  </si>
+  <si>
+    <t>Saved model_cnn1_3.h5py as  model_cnn1_5.h5py. May need to continue</t>
+  </si>
+  <si>
+    <t>"relu"</t>
+  </si>
+  <si>
+    <t>both are very bad</t>
+  </si>
+  <si>
+    <t>Not good</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>4_1; 4_2 not good</t>
+  </si>
+  <si>
+    <t>5 were not good</t>
+  </si>
+  <si>
+    <t>2_1; 2_2 =&gt; are good. 2_3 run another =&gt; alright; 2_4 run another not good</t>
+  </si>
+  <si>
+    <t>model_cnn2_2.h5py / model_cnn2_1.h5py /  model_cnn2_3.h5py</t>
+  </si>
+  <si>
+    <t>1_10 so so; 1_11 not good</t>
+  </si>
+  <si>
+    <t>2_10 not that bad but could be better. 2_11 is so so, continued bad as well</t>
+  </si>
+  <si>
+    <t>continuation of 2_11</t>
+  </si>
+  <si>
+    <t>"selu"</t>
+  </si>
+  <si>
+    <t>selu+linear</t>
+  </si>
+  <si>
+    <t>modified CNN4 significantly</t>
+  </si>
+  <si>
+    <t>case4_1</t>
+  </si>
+  <si>
+    <t>case4_2</t>
+  </si>
+  <si>
+    <t>case4_3</t>
+  </si>
+  <si>
+    <t>case4_4</t>
+  </si>
+  <si>
+    <t>case4_5</t>
+  </si>
+  <si>
+    <t>case2_1</t>
+  </si>
+  <si>
+    <t>case2_2</t>
+  </si>
+  <si>
+    <t>case2_3</t>
+  </si>
+  <si>
+    <t>case2_4</t>
+  </si>
+  <si>
+    <t>case2_5</t>
+  </si>
+  <si>
+    <t>case1_1</t>
+  </si>
+  <si>
+    <t>"selu"+ linear</t>
+  </si>
+  <si>
+    <t>Saved</t>
+  </si>
+  <si>
+    <t>saved model_cnn1_1.h5py</t>
+  </si>
+  <si>
+    <t>case1_2</t>
+  </si>
+  <si>
+    <t>case1_3</t>
+  </si>
+  <si>
+    <t>case1_4</t>
+  </si>
+  <si>
+    <t>case1_5</t>
+  </si>
+  <si>
+    <t>Linux</t>
   </si>
 </sst>
 </file>
@@ -209,20 +300,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -505,58 +621,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:Q19"/>
+  <dimension ref="B3:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="59.44140625" customWidth="1"/>
-    <col min="9" max="9" width="31.109375" customWidth="1"/>
-    <col min="10" max="10" width="39.6640625" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="60.109375" customWidth="1"/>
+    <col min="10" max="10" width="32.88671875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>809914</v>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -564,22 +683,17 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>809915</v>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -587,16 +701,21 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>809918</v>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -605,16 +724,16 @@
         <v>3</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>809804</v>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -622,16 +741,17 @@
       <c r="D7" s="1">
         <v>4</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>809906</v>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -642,137 +762,551 @@
       <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+    </row>
+    <row r="13" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G9" s="3"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G10" s="3"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>810164</v>
+      <c r="I13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>810163</v>
+        <v>41</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="1">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G18" s="1"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>810174</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>810175</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>36</v>
+      <c r="I23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="12">
+        <v>811157</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="1">
+        <v>4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>811158</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>811159</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>811160</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4</v>
+      </c>
+      <c r="E28" s="1">
+        <v>4</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>811161</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1">
+        <v>4</v>
+      </c>
+      <c r="E29" s="1">
+        <v>5</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>811162</v>
+      </c>
+      <c r="C31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>811163</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>811164</v>
+      </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>811165</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>811166</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>5</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>811174</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>811175</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>2</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>811176</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>811177</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>4</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>811178</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>5</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="J12:Q12"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="K12:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modified back cnn1 architecture
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD23BAF-7F4B-42E3-B2C4-571C68A9CEDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C00D265-66D0-4EED-BB2D-4C0D624D2A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="94">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -238,13 +238,82 @@
   </si>
   <si>
     <t>Linux</t>
+  </si>
+  <si>
+    <t>case6_2</t>
+  </si>
+  <si>
+    <t>case6_1</t>
+  </si>
+  <si>
+    <t>case6_3</t>
+  </si>
+  <si>
+    <t>case6_4</t>
+  </si>
+  <si>
+    <t>case6_5</t>
+  </si>
+  <si>
+    <t>NO Keras augmentation rotation</t>
+  </si>
+  <si>
+    <t>not good</t>
+  </si>
+  <si>
+    <t>more or less ok</t>
+  </si>
+  <si>
+    <t>case1_6</t>
+  </si>
+  <si>
+    <t>case1_7</t>
+  </si>
+  <si>
+    <t>case1_8</t>
+  </si>
+  <si>
+    <t>case1_9</t>
+  </si>
+  <si>
+    <t>modified back the CNN, see Report 66.1</t>
+  </si>
+  <si>
+    <t>modified back the CNN, see Report 66.2</t>
+  </si>
+  <si>
+    <t>modified back the CNN, see Report 66.3</t>
+  </si>
+  <si>
+    <t>modified back the CNN, see Report 66.4</t>
+  </si>
+  <si>
+    <t>case1_10</t>
+  </si>
+  <si>
+    <t>modified back the CNN, see Report 66.5</t>
+  </si>
+  <si>
+    <t>case6_6</t>
+  </si>
+  <si>
+    <t>case6_7</t>
+  </si>
+  <si>
+    <t>case6_8</t>
+  </si>
+  <si>
+    <t>case6_9</t>
+  </si>
+  <si>
+    <t>case6_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +338,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -338,9 +413,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,27 +700,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R42"/>
+  <dimension ref="B3:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
     <col min="9" max="9" width="60.109375" customWidth="1"/>
     <col min="10" max="10" width="32.88671875" style="6" customWidth="1"/>
     <col min="11" max="11" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -673,641 +753,985 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J11" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-    </row>
-    <row r="13" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1">
-        <v>4</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>811209</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="H14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>14</v>
+        <v>38</v>
+      </c>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>811208</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="H15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>811207</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>811206</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G18" s="13"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G19" s="13"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+    </row>
+    <row r="21" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C24" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D24" s="1">
         <v>2</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E24" s="1">
         <v>11</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="11" t="s">
+      <c r="F24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I24" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J24" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C25" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="11" t="s">
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I25" t="s">
         <v>65</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G18" s="1"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G26" s="1"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C28" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J28" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="29" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C29" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D29" s="1">
         <v>2</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J29" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>70</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C30" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D30" s="1">
         <v>3</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J30" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D31" s="1">
         <v>3</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J31" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="12">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="12">
         <v>811157</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C33" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D33" s="1">
         <v>4</v>
       </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34">
         <v>811158</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C34" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D34" s="1">
         <v>4</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E34" s="1">
         <v>2</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27">
+      <c r="G34" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35">
         <v>811159</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C35" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D35" s="1">
         <v>4</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E35" s="1">
         <v>3</v>
       </c>
-      <c r="G27" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28">
+      <c r="G35" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36">
         <v>811160</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C36" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D36" s="1">
         <v>4</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E36" s="1">
         <v>4</v>
       </c>
-      <c r="G28" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29">
+      <c r="G36" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B37">
         <v>811161</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C37" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D37" s="1">
         <v>4</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E37" s="1">
         <v>5</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31">
+      <c r="G37" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39">
         <v>811162</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C39" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D39" s="1">
         <v>2</v>
       </c>
-      <c r="E31" s="1">
-        <v>1</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="11" t="s">
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32">
+      <c r="J39" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40">
         <v>811163</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C40" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D40" s="1">
         <v>2</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E40" s="1">
         <v>2</v>
       </c>
-      <c r="G32" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="11" t="s">
+      <c r="G40" s="13"/>
+      <c r="H40" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33">
+      <c r="J40" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41">
         <v>811164</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C41" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D41" s="1">
         <v>2</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E41" s="1">
         <v>3</v>
       </c>
-      <c r="G33" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="11" t="s">
+      <c r="G41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B42">
         <v>811165</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C42" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D42" s="1">
         <v>2</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E42" s="1">
         <v>4</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="11" t="s">
+      <c r="G42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43">
         <v>811166</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C43" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D43" s="1">
         <v>2</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E43" s="1">
         <v>5</v>
       </c>
-      <c r="G35" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="11" t="s">
+      <c r="G43" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B46">
         <v>811174</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C46" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="1">
-        <v>1</v>
-      </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="11" t="s">
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39">
+      <c r="J46" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B47">
         <v>811175</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C47" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1">
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
         <v>2</v>
       </c>
-      <c r="G39" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="11" t="s">
+      <c r="G47" s="13"/>
+      <c r="H47" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40">
+      <c r="J47" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B48">
         <v>811176</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C48" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="1">
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1">
         <v>3</v>
       </c>
-      <c r="G40" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="11" t="s">
+      <c r="G48" s="13"/>
+      <c r="H48" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41">
+      <c r="J48" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49">
         <v>811177</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C49" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1">
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
         <v>4</v>
       </c>
-      <c r="G41" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="11" t="s">
+      <c r="G49" s="13"/>
+      <c r="H49" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42">
+      <c r="J49" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50">
         <v>811178</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C50" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="1">
-        <v>1</v>
-      </c>
-      <c r="E42" s="1">
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
         <v>5</v>
       </c>
-      <c r="G42" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="11" t="s">
+      <c r="G50" s="13"/>
+      <c r="H50" s="11" t="s">
         <v>49</v>
       </c>
+      <c r="J50" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>811212</v>
+      </c>
+      <c r="C52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>6</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>811213</v>
+      </c>
+      <c r="C53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1">
+        <v>7</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>811214</v>
+      </c>
+      <c r="C54" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1">
+        <v>8</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I54" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>811215</v>
+      </c>
+      <c r="C55" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1">
+        <v>9</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>811216</v>
+      </c>
+      <c r="C56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1">
+        <v>10</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>811217</v>
+      </c>
+      <c r="C58" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="1">
+        <v>6</v>
+      </c>
+      <c r="E58" s="1">
+        <v>6</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>811218</v>
+      </c>
+      <c r="C59" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="1">
+        <v>6</v>
+      </c>
+      <c r="E59" s="1">
+        <v>7</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>811219</v>
+      </c>
+      <c r="C60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60" s="1">
+        <v>6</v>
+      </c>
+      <c r="E60" s="1">
+        <v>8</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>811220</v>
+      </c>
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="1">
+        <v>6</v>
+      </c>
+      <c r="E61" s="1">
+        <v>9</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>811221</v>
+      </c>
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="1">
+        <v>6</v>
+      </c>
+      <c r="E62" s="1">
+        <v>10</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="K12:R12"/>
+  <mergeCells count="3">
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="B6:J6"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Good results from CNN6 modified a bit architecture
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C00D265-66D0-4EED-BB2D-4C0D624D2A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7537F8-9B59-4EA6-B230-A088E7DBD0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>case6_10</t>
+  </si>
+  <si>
+    <t>case6_11</t>
+  </si>
+  <si>
+    <t>Added one line of dense at the final</t>
+  </si>
+  <si>
+    <t>good results, saved</t>
   </si>
 </sst>
 </file>
@@ -413,13 +422,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R62"/>
+  <dimension ref="B3:R63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,20 +762,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -984,25 +993,25 @@
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
     </row>
     <row r="21" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
@@ -1723,6 +1732,30 @@
       </c>
       <c r="H62" s="11" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="s">
+        <v>94</v>
+      </c>
+      <c r="D63" s="1">
+        <v>6</v>
+      </c>
+      <c r="E63" s="1">
+        <v>10</v>
+      </c>
+      <c r="G63" s="13"/>
+      <c r="H63" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I63" t="s">
+        <v>95</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added function to load and plot my CVSfile results of the running,
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7537F8-9B59-4EA6-B230-A088E7DBD0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A466FE6A-9EAE-4A69-85C8-F923BA9C3415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -312,10 +312,22 @@
     <t>case6_11</t>
   </si>
   <si>
-    <t>Added one line of dense at the final</t>
-  </si>
-  <si>
     <t>good results, saved</t>
+  </si>
+  <si>
+    <t>CNN: added one line of dense at the final</t>
+  </si>
+  <si>
+    <t>case6_12</t>
+  </si>
+  <si>
+    <t>case6_13</t>
+  </si>
+  <si>
+    <t>case6_14</t>
+  </si>
+  <si>
+    <t>case6_15</t>
   </si>
 </sst>
 </file>
@@ -709,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R63"/>
+  <dimension ref="B3:R69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,9 +906,7 @@
       <c r="E13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G13" s="13"/>
       <c r="H13" s="11" t="s">
         <v>38</v>
       </c>
@@ -936,9 +946,7 @@
       <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G15" s="13"/>
       <c r="H15" s="11" t="s">
         <v>38</v>
       </c>
@@ -1734,29 +1742,124 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
         <v>14</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>94</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D64" s="1">
         <v>6</v>
       </c>
-      <c r="E63" s="1">
-        <v>10</v>
-      </c>
-      <c r="G63" s="13"/>
-      <c r="H63" s="11" t="s">
+      <c r="E64" s="1">
+        <v>11</v>
+      </c>
+      <c r="G64" s="13"/>
+      <c r="H64" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I64" t="s">
+        <v>96</v>
+      </c>
+      <c r="J64" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="J63" s="8" t="s">
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>811228</v>
+      </c>
+      <c r="C65" t="s">
+        <v>97</v>
+      </c>
+      <c r="D65" s="1">
+        <v>6</v>
+      </c>
+      <c r="E65" s="1">
+        <v>12</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I65" t="s">
         <v>96</v>
       </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>811229</v>
+      </c>
+      <c r="C66" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" s="1">
+        <v>6</v>
+      </c>
+      <c r="E66" s="1">
+        <v>13</v>
+      </c>
+      <c r="G66" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>811233</v>
+      </c>
+      <c r="C67" t="s">
+        <v>99</v>
+      </c>
+      <c r="D67" s="1">
+        <v>6</v>
+      </c>
+      <c r="E67" s="1">
+        <v>14</v>
+      </c>
+      <c r="G67" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>811232</v>
+      </c>
+      <c r="C68" t="s">
+        <v>100</v>
+      </c>
+      <c r="D68" s="1">
+        <v>6</v>
+      </c>
+      <c r="E68" s="1">
+        <v>15</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H69" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Small dataname mistake in the previous commit, can give error when testing. Corrected.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A466FE6A-9EAE-4A69-85C8-F923BA9C3415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F3B44-13D1-44E8-A75E-2059996D5342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -328,13 +328,43 @@
   </si>
   <si>
     <t>case6_15</t>
+  </si>
+  <si>
+    <t>Bald data</t>
+  </si>
+  <si>
+    <t>Not bad!</t>
+  </si>
+  <si>
+    <t>model_cnn2_12.h5py</t>
+  </si>
+  <si>
+    <t>case6_16</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CNN: added one line of dense at the final. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bald data</t>
+    </r>
+  </si>
+  <si>
+    <t>model_cnn6_11.h5py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,6 +399,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -396,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,6 +476,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -721,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R69"/>
+  <dimension ref="B3:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,8 +775,8 @@
     <col min="4" max="4" width="5.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
     <col min="9" max="9" width="60.109375" customWidth="1"/>
     <col min="10" max="10" width="32.88671875" style="6" customWidth="1"/>
     <col min="11" max="11" width="54.77734375" customWidth="1"/>
@@ -997,72 +1037,62 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>12</v>
+      </c>
       <c r="G19" s="13"/>
-      <c r="H19" s="11"/>
+      <c r="H19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="s">
+      <c r="G20" s="13"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G21" s="13"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-    </row>
-    <row r="21" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="1">
-        <v>4</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+    </row>
+    <row r="23" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>14</v>
       </c>
@@ -1070,20 +1100,16 @@
         <v>15</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="11" t="s">
-        <v>38</v>
+        <v>4</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -1091,23 +1117,20 @@
         <v>15</v>
       </c>
       <c r="D24" s="1">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>11</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" t="s">
-        <v>48</v>
+        <v>34</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
@@ -1120,184 +1143,198 @@
       <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="E25" s="1">
-        <v>1</v>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" t="s">
         <v>65</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J27" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G26" s="1"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D30" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D31" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J32" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J33" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="12">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="12">
         <v>811157</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>52</v>
-      </c>
-      <c r="D33" s="1">
-        <v>4</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34">
-        <v>811158</v>
-      </c>
-      <c r="C34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="1">
-        <v>4</v>
-      </c>
-      <c r="E34" s="1">
-        <v>2</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35">
-        <v>811159</v>
-      </c>
-      <c r="C35" t="s">
-        <v>54</v>
       </c>
       <c r="D35" s="1">
         <v>4</v>
       </c>
       <c r="E35" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>7</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36">
-        <v>811160</v>
+        <v>811158</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D36" s="1">
         <v>4</v>
       </c>
       <c r="E36" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>7</v>
@@ -1305,115 +1342,109 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37">
-        <v>811161</v>
+        <v>811159</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1">
         <v>4</v>
       </c>
       <c r="E37" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G37" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>811160</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4</v>
+      </c>
+      <c r="E38" s="1">
+        <v>4</v>
+      </c>
+      <c r="G38" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39">
-        <v>811162</v>
+        <v>811161</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E39" s="1">
-        <v>1</v>
-      </c>
-      <c r="G39" s="13"/>
-      <c r="H39" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40">
-        <v>811163</v>
-      </c>
-      <c r="C40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40" s="1">
-        <v>2</v>
-      </c>
-      <c r="E40" s="1">
-        <v>2</v>
-      </c>
-      <c r="G40" s="13"/>
-      <c r="H40" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>77</v>
+        <v>5</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41">
-        <v>811164</v>
+        <v>811162</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D41" s="1">
         <v>2</v>
       </c>
       <c r="E41" s="1">
-        <v>3</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G41" s="13"/>
       <c r="H41" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="J41" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42">
-        <v>811165</v>
+        <v>811163</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D42" s="1">
         <v>2</v>
       </c>
       <c r="E42" s="1">
-        <v>4</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>7</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G42" s="13"/>
       <c r="H42" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="J42" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43">
-        <v>811166</v>
+        <v>811164</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D43" s="1">
         <v>2</v>
       </c>
       <c r="E43" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>7</v>
@@ -1422,60 +1453,58 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B46">
-        <v>811174</v>
-      </c>
-      <c r="C46" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
-      <c r="E46" s="1">
-        <v>1</v>
-      </c>
-      <c r="G46" s="13"/>
-      <c r="H46" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47">
-        <v>811175</v>
-      </c>
-      <c r="C47" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>811165</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="1">
         <v>2</v>
       </c>
-      <c r="G47" s="13"/>
-      <c r="H47" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>77</v>
+      <c r="E44" s="1">
+        <v>4</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>811166</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>5</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48">
-        <v>811176</v>
+        <v>811174</v>
       </c>
       <c r="C48" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
       <c r="E48" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G48" s="13"/>
       <c r="H48" s="11" t="s">
@@ -1487,37 +1516,37 @@
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49">
-        <v>811177</v>
+        <v>811175</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
       <c r="E49" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G49" s="13"/>
       <c r="H49" s="11" t="s">
         <v>49</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50">
-        <v>811178</v>
+        <v>811176</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G50" s="13"/>
       <c r="H50" s="11" t="s">
@@ -1527,64 +1556,60 @@
         <v>77</v>
       </c>
     </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>811177</v>
+      </c>
+      <c r="C51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1">
+        <v>4</v>
+      </c>
+      <c r="G51" s="13"/>
+      <c r="H51" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52">
-        <v>811212</v>
+        <v>811178</v>
       </c>
       <c r="C52" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
       <c r="E52" s="1">
-        <v>6</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G52" s="13"/>
       <c r="H52" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I52" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53">
-        <v>811213</v>
-      </c>
-      <c r="C53" t="s">
-        <v>80</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1">
-        <v>7</v>
-      </c>
-      <c r="G53" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I53" t="s">
-        <v>84</v>
+      <c r="J52" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54">
-        <v>811214</v>
+        <v>811212</v>
       </c>
       <c r="C54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
       </c>
       <c r="E54" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G54" s="13" t="s">
         <v>7</v>
@@ -1593,21 +1618,21 @@
         <v>49</v>
       </c>
       <c r="I54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55">
-        <v>811215</v>
+        <v>811213</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
       </c>
       <c r="E55" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>7</v>
@@ -1616,21 +1641,21 @@
         <v>49</v>
       </c>
       <c r="I55" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56">
-        <v>811216</v>
+        <v>811214</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
       </c>
       <c r="E56" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>7</v>
@@ -1639,61 +1664,67 @@
         <v>49</v>
       </c>
       <c r="I56" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>811215</v>
+      </c>
+      <c r="C57" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1">
+        <v>9</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I57" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58">
-        <v>811217</v>
+        <v>811216</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D58" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E58" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B59">
-        <v>811218</v>
-      </c>
-      <c r="C59" t="s">
-        <v>90</v>
-      </c>
-      <c r="D59" s="1">
-        <v>6</v>
-      </c>
-      <c r="E59" s="1">
-        <v>7</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="I58" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60">
-        <v>811219</v>
+        <v>811217</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D60" s="1">
         <v>6</v>
       </c>
       <c r="E60" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>7</v>
@@ -1704,16 +1735,16 @@
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61">
-        <v>811220</v>
+        <v>811218</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D61" s="1">
         <v>6</v>
       </c>
       <c r="E61" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>7</v>
@@ -1724,16 +1755,16 @@
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B62">
-        <v>811221</v>
+        <v>811219</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D62" s="1">
         <v>6</v>
       </c>
       <c r="E62" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>7</v>
@@ -1742,88 +1773,85 @@
         <v>38</v>
       </c>
     </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>811220</v>
+      </c>
+      <c r="C63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="1">
+        <v>6</v>
+      </c>
+      <c r="E63" s="1">
+        <v>9</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
-        <v>14</v>
+      <c r="B64">
+        <v>811221</v>
       </c>
       <c r="C64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D64" s="1">
         <v>6</v>
       </c>
       <c r="E64" s="1">
-        <v>11</v>
-      </c>
-      <c r="G64" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="H64" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I64" t="s">
-        <v>96</v>
-      </c>
-      <c r="J64" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B65">
-        <v>811228</v>
-      </c>
-      <c r="C65" t="s">
-        <v>97</v>
-      </c>
-      <c r="D65" s="1">
-        <v>6</v>
-      </c>
-      <c r="E65" s="1">
-        <v>12</v>
-      </c>
-      <c r="G65" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H65" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I65" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B66">
-        <v>811229</v>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D66" s="1">
         <v>6</v>
       </c>
       <c r="E66" s="1">
-        <v>13</v>
-      </c>
-      <c r="G66" s="13" t="s">
-        <v>7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G66" s="13"/>
       <c r="H66" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I66" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J66" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K66" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B67">
-        <v>811233</v>
+        <v>811228</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D67" s="1">
         <v>6</v>
       </c>
       <c r="E67" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>7</v>
@@ -1835,18 +1863,18 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B68">
-        <v>811232</v>
+        <v>811229</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D68" s="1">
         <v>6</v>
       </c>
       <c r="E68" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>7</v>
@@ -1858,13 +1886,79 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H69" s="11"/>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>811233</v>
+      </c>
+      <c r="C69" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="1">
+        <v>6</v>
+      </c>
+      <c r="E69" s="1">
+        <v>14</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>811232</v>
+      </c>
+      <c r="C70" t="s">
+        <v>100</v>
+      </c>
+      <c r="D70" s="1">
+        <v>6</v>
+      </c>
+      <c r="E70" s="1">
+        <v>15</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I70" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" t="s">
+        <v>104</v>
+      </c>
+      <c r="D72" s="1">
+        <v>6</v>
+      </c>
+      <c r="E72" s="1">
+        <v>16</v>
+      </c>
+      <c r="G72" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I72" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="K22:R22"/>
     <mergeCell ref="B6:J6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Shuffled things to correct places, and improved the code a bit.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F3B44-13D1-44E8-A75E-2059996D5342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C1CA5A-5683-474F-B63C-C91B8F99057C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="64000data" sheetId="1" r:id="rId1"/>
+    <sheet name="64000 Bald data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="116">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -279,21 +280,9 @@
     <t>modified back the CNN, see Report 66.1</t>
   </si>
   <si>
-    <t>modified back the CNN, see Report 66.2</t>
-  </si>
-  <si>
-    <t>modified back the CNN, see Report 66.3</t>
-  </si>
-  <si>
-    <t>modified back the CNN, see Report 66.4</t>
-  </si>
-  <si>
     <t>case1_10</t>
   </si>
   <si>
-    <t>modified back the CNN, see Report 66.5</t>
-  </si>
-  <si>
     <t>case6_6</t>
   </si>
   <si>
@@ -337,9 +326,6 @@
   </si>
   <si>
     <t>model_cnn2_12.h5py</t>
-  </si>
-  <si>
-    <t>case6_16</t>
   </si>
   <si>
     <r>
@@ -358,6 +344,48 @@
   </si>
   <si>
     <t>model_cnn6_11.h5py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not too bad, but worse than model_cnn1_1.h5py </t>
+  </si>
+  <si>
+    <t>I think it can be inmpoved</t>
+  </si>
+  <si>
+    <t>case6_17</t>
+  </si>
+  <si>
+    <t>case6_18</t>
+  </si>
+  <si>
+    <t>case6_19</t>
+  </si>
+  <si>
+    <t>case6_20</t>
+  </si>
+  <si>
+    <t>Augment</t>
+  </si>
+  <si>
+    <t>case2_13</t>
+  </si>
+  <si>
+    <t>case2_14</t>
+  </si>
+  <si>
+    <t>case2_15</t>
+  </si>
+  <si>
+    <t>case2_16</t>
+  </si>
+  <si>
+    <t>leakyRELU-linear</t>
+  </si>
+  <si>
+    <t>not good visually, despite low mape 7%</t>
+  </si>
+  <si>
+    <t>worse than 6_11, thus deleted</t>
   </si>
 </sst>
 </file>
@@ -433,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -472,13 +500,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -761,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R72"/>
+  <dimension ref="B3:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,7 +809,7 @@
     <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" customWidth="1"/>
     <col min="9" max="9" width="60.109375" customWidth="1"/>
-    <col min="10" max="10" width="32.88671875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="34.6640625" style="6" customWidth="1"/>
     <col min="11" max="11" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -817,17 +848,17 @@
     <row r="4" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -965,13 +996,13 @@
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15">
@@ -1036,33 +1067,6 @@
       <c r="G18" s="13"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1">
-        <v>12</v>
-      </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="G20" s="13"/>
       <c r="H20" s="11"/>
@@ -1072,25 +1076,25 @@
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
     </row>
     <row r="23" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
@@ -1446,11 +1450,12 @@
       <c r="E43" s="1">
         <v>3</v>
       </c>
-      <c r="G43" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G43" s="13"/>
       <c r="H43" s="11" t="s">
         <v>63</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
@@ -1466,11 +1471,12 @@
       <c r="E44" s="1">
         <v>4</v>
       </c>
-      <c r="G44" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G44" s="13"/>
       <c r="H44" s="11" t="s">
         <v>63</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
@@ -1486,11 +1492,12 @@
       <c r="E45" s="1">
         <v>5</v>
       </c>
-      <c r="G45" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G45" s="13"/>
       <c r="H45" s="11" t="s">
         <v>63</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
@@ -1598,7 +1605,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>811212</v>
       </c>
@@ -1611,17 +1618,18 @@
       <c r="E54" s="1">
         <v>6</v>
       </c>
-      <c r="G54" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G54" s="13"/>
       <c r="H54" s="11" t="s">
         <v>49</v>
       </c>
       <c r="I54" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J54" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>811213</v>
       </c>
@@ -1634,17 +1642,18 @@
       <c r="E55" s="1">
         <v>7</v>
       </c>
-      <c r="G55" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G55" s="13"/>
       <c r="H55" s="11" t="s">
         <v>49</v>
       </c>
       <c r="I55" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>811214</v>
       </c>
@@ -1657,14 +1666,15 @@
       <c r="E56" s="1">
         <v>8</v>
       </c>
-      <c r="G56" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G56" s="13"/>
       <c r="H56" s="11" t="s">
         <v>49</v>
       </c>
       <c r="I56" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
@@ -1687,7 +1697,7 @@
         <v>49</v>
       </c>
       <c r="I57" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
@@ -1695,7 +1705,7 @@
         <v>811216</v>
       </c>
       <c r="C58" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
@@ -1710,7 +1720,7 @@
         <v>49</v>
       </c>
       <c r="I58" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.3">
@@ -1718,7 +1728,7 @@
         <v>811217</v>
       </c>
       <c r="C60" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D60" s="1">
         <v>6</v>
@@ -1738,7 +1748,7 @@
         <v>811218</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D61" s="1">
         <v>6</v>
@@ -1758,7 +1768,7 @@
         <v>811219</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D62" s="1">
         <v>6</v>
@@ -1778,7 +1788,7 @@
         <v>811220</v>
       </c>
       <c r="C63" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D63" s="1">
         <v>6</v>
@@ -1798,7 +1808,7 @@
         <v>811221</v>
       </c>
       <c r="C64" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D64" s="1">
         <v>6</v>
@@ -1818,7 +1828,7 @@
         <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D66" s="1">
         <v>6</v>
@@ -1831,13 +1841,13 @@
         <v>38</v>
       </c>
       <c r="I66" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K66" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.3">
@@ -1845,7 +1855,7 @@
         <v>811228</v>
       </c>
       <c r="C67" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D67" s="1">
         <v>6</v>
@@ -1860,7 +1870,7 @@
         <v>38</v>
       </c>
       <c r="I67" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.3">
@@ -1868,7 +1878,7 @@
         <v>811229</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D68" s="1">
         <v>6</v>
@@ -1883,15 +1893,15 @@
         <v>38</v>
       </c>
       <c r="I68" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>811233</v>
       </c>
       <c r="C69" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D69" s="1">
         <v>6</v>
@@ -1899,14 +1909,15 @@
       <c r="E69" s="1">
         <v>14</v>
       </c>
-      <c r="G69" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G69" s="13"/>
       <c r="H69" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I69" t="s">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.3">
@@ -1914,7 +1925,7 @@
         <v>811232</v>
       </c>
       <c r="C70" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D70" s="1">
         <v>6</v>
@@ -1922,37 +1933,15 @@
       <c r="E70" s="1">
         <v>15</v>
       </c>
-      <c r="G70" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G70" s="13"/>
       <c r="H70" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I70" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
-        <v>14</v>
-      </c>
-      <c r="C72" t="s">
-        <v>104</v>
-      </c>
-      <c r="D72" s="1">
-        <v>6</v>
-      </c>
-      <c r="E72" s="1">
-        <v>16</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H72" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I72" t="s">
-        <v>105</v>
+        <v>92</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1965,4 +1954,306 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
+  <dimension ref="B3:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="43.109375" customWidth="1"/>
+    <col min="10" max="10" width="24.21875" customWidth="1"/>
+    <col min="11" max="11" width="27.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>811258</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>13</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>811259</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>14</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>811260</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>15</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>811261</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>16</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>811254</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1">
+        <v>17</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>811255</v>
+      </c>
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1">
+        <v>18</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>811256</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>19</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>811257</v>
+      </c>
+      <c r="C16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>20</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified data engineering part => for the new 75110 images
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C1CA5A-5683-474F-B63C-C91B8F99057C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EAA641-5AD8-474C-BF5C-58F42C230094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="64000data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="127">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -320,9 +320,6 @@
   </si>
   <si>
     <t>Bald data</t>
-  </si>
-  <si>
-    <t>Not bad!</t>
   </si>
   <si>
     <t>model_cnn2_12.h5py</t>
@@ -349,9 +346,6 @@
     <t xml:space="preserve">not too bad, but worse than model_cnn1_1.h5py </t>
   </si>
   <si>
-    <t>I think it can be inmpoved</t>
-  </si>
-  <si>
     <t>case6_17</t>
   </si>
   <si>
@@ -386,6 +380,45 @@
   </si>
   <si>
     <t>worse than 6_11, thus deleted</t>
+  </si>
+  <si>
+    <t>I think it can be impoved</t>
+  </si>
+  <si>
+    <t>best among 2</t>
+  </si>
+  <si>
+    <t>Best among 5</t>
+  </si>
+  <si>
+    <t>TRUE?</t>
+  </si>
+  <si>
+    <t>Best among 5, but worse than 6_11</t>
+  </si>
+  <si>
+    <t>3.1 days runtime linux. Because of alarm?</t>
+  </si>
+  <si>
+    <t>1.8 days runtime linux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good more or less. Maybe better slightly than model_cnn1_1.h5py  </t>
+  </si>
+  <si>
+    <t>model_cnn1_10.h5py</t>
+  </si>
+  <si>
+    <t>ResNet50</t>
+  </si>
+  <si>
+    <t>model_cnn6_4.h5py</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">425505 Bus error               (core dumped) </t>
   </si>
 </sst>
 </file>
@@ -461,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,6 +539,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,17 +882,17 @@
     <row r="4" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -981,6 +1015,9 @@
       <c r="H13" s="11" t="s">
         <v>38</v>
       </c>
+      <c r="I13" t="s">
+        <v>123</v>
+      </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -1000,6 +1037,9 @@
       <c r="H14" s="11" t="s">
         <v>38</v>
       </c>
+      <c r="I14" t="s">
+        <v>123</v>
+      </c>
       <c r="J14" s="9" t="s">
         <v>40</v>
       </c>
@@ -1021,6 +1061,9 @@
       <c r="H15" s="11" t="s">
         <v>38</v>
       </c>
+      <c r="I15" t="s">
+        <v>123</v>
+      </c>
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -1036,11 +1079,18 @@
       <c r="E16" s="1">
         <v>4</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G16" s="13"/>
       <c r="H16" s="11" t="s">
         <v>38</v>
+      </c>
+      <c r="I16" t="s">
+        <v>123</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
@@ -1056,11 +1106,15 @@
       <c r="E17" s="1">
         <v>5</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G17" s="13"/>
       <c r="H17" s="11" t="s">
         <v>38</v>
+      </c>
+      <c r="I17" t="s">
+        <v>123</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
@@ -1076,25 +1130,25 @@
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
     </row>
     <row r="23" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
@@ -1357,8 +1411,11 @@
       <c r="E37" s="1">
         <v>3</v>
       </c>
-      <c r="G37" s="13" t="s">
-        <v>7</v>
+      <c r="G37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I37" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
@@ -1374,8 +1431,11 @@
       <c r="E38" s="1">
         <v>4</v>
       </c>
-      <c r="G38" s="13" t="s">
-        <v>7</v>
+      <c r="G38" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I38" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
@@ -1391,8 +1451,11 @@
       <c r="E39" s="1">
         <v>5</v>
       </c>
-      <c r="G39" s="13" t="s">
-        <v>7</v>
+      <c r="G39" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I39" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
@@ -1521,7 +1584,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>811175</v>
       </c>
@@ -1542,7 +1605,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>811176</v>
       </c>
@@ -1563,7 +1626,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>811177</v>
       </c>
@@ -1584,7 +1647,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>811178</v>
       </c>
@@ -1605,7 +1668,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>811212</v>
       </c>
@@ -1626,10 +1689,10 @@
         <v>83</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>811213</v>
       </c>
@@ -1650,10 +1713,10 @@
         <v>83</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>811214</v>
       </c>
@@ -1674,10 +1737,10 @@
         <v>83</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>811215</v>
       </c>
@@ -1690,17 +1753,18 @@
       <c r="E57" s="1">
         <v>9</v>
       </c>
-      <c r="G57" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G57" s="13"/>
       <c r="H57" s="11" t="s">
         <v>49</v>
       </c>
       <c r="I57" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J57" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>811216</v>
       </c>
@@ -1713,17 +1777,21 @@
       <c r="E58" s="1">
         <v>10</v>
       </c>
-      <c r="G58" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G58" s="13"/>
       <c r="H58" s="11" t="s">
         <v>49</v>
       </c>
       <c r="I58" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J58" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B60">
         <v>811217</v>
       </c>
@@ -1736,14 +1804,15 @@
       <c r="E60" s="1">
         <v>6</v>
       </c>
-      <c r="G60" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G60" s="13"/>
       <c r="H60" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>811218</v>
       </c>
@@ -1756,14 +1825,12 @@
       <c r="E61" s="1">
         <v>7</v>
       </c>
-      <c r="G61" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G61" s="13"/>
       <c r="H61" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>811219</v>
       </c>
@@ -1776,14 +1843,18 @@
       <c r="E62" s="1">
         <v>8</v>
       </c>
-      <c r="G62" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G62" s="13"/>
       <c r="H62" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I62" t="s">
+        <v>120</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>811220</v>
       </c>
@@ -1796,14 +1867,12 @@
       <c r="E63" s="1">
         <v>9</v>
       </c>
-      <c r="G63" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G63" s="13"/>
       <c r="H63" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>811221</v>
       </c>
@@ -1816,9 +1885,7 @@
       <c r="E64" s="1">
         <v>10</v>
       </c>
-      <c r="G64" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G64" s="13"/>
       <c r="H64" s="11" t="s">
         <v>38</v>
       </c>
@@ -1847,7 +1914,7 @@
         <v>91</v>
       </c>
       <c r="K66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.3">
@@ -1917,7 +1984,7 @@
         <v>92</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.3">
@@ -1941,7 +2008,7 @@
         <v>92</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1960,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
   <dimension ref="B3:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,7 +2056,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>10</v>
@@ -2020,19 +2087,21 @@
       <c r="E4" s="1">
         <v>12</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="G4" s="13"/>
       <c r="H4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
@@ -2040,7 +2109,7 @@
         <v>811258</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -2051,11 +2120,12 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G5" s="13"/>
       <c r="H5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
@@ -2063,7 +2133,7 @@
         <v>811259</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
@@ -2074,11 +2144,12 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G6" s="13"/>
       <c r="H6" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -2086,7 +2157,7 @@
         <v>811260</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -2097,11 +2168,12 @@
       <c r="F7" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G7" s="13"/>
       <c r="H7" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
@@ -2109,7 +2181,7 @@
         <v>811261</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
@@ -2120,11 +2192,12 @@
       <c r="F8" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G8" s="13"/>
       <c r="H8" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
@@ -2154,10 +2227,10 @@
         <v>38</v>
       </c>
       <c r="I12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J12" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
@@ -2165,7 +2238,7 @@
         <v>811254</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D13" s="1">
         <v>6</v>
@@ -2176,9 +2249,7 @@
       <c r="F13" t="b">
         <v>1</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G13" s="13"/>
       <c r="H13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2188,7 +2259,7 @@
         <v>811255</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D14" s="1">
         <v>6</v>
@@ -2199,11 +2270,12 @@
       <c r="F14" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="11" t="s">
         <v>38</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -2211,7 +2283,7 @@
         <v>811256</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -2234,7 +2306,7 @@
         <v>811257</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D16" s="1">
         <v>6</v>
@@ -2255,5 +2327,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Improved path names - Added canceling multi-threading in linux
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,25 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EAA641-5AD8-474C-BF5C-58F42C230094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2C6CD1-ECFE-42A8-AEF2-6F3C02C78426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="64000data" sheetId="1" r:id="rId1"/>
     <sheet name="64000 Bald data" sheetId="2" r:id="rId2"/>
+    <sheet name="300440data" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="133">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -419,6 +428,24 @@
   </si>
   <si>
     <t xml:space="preserve">425505 Bus error               (core dumped) </t>
+  </si>
+  <si>
+    <t>case2_20</t>
+  </si>
+  <si>
+    <t>case2_21</t>
+  </si>
+  <si>
+    <t>case2_22</t>
+  </si>
+  <si>
+    <t>case2_23</t>
+  </si>
+  <si>
+    <t>case2_24</t>
+  </si>
+  <si>
+    <t>case2_25</t>
   </si>
 </sst>
 </file>
@@ -494,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -540,6 +567,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -828,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R70"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,17 +912,17 @@
     <row r="4" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -1130,25 +1160,25 @@
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
     </row>
     <row r="23" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
@@ -2027,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
   <dimension ref="B3:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2329,4 +2359,169 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1723D785-94D7-412E-814C-F8487739E257}">
+  <dimension ref="B2:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="10" max="10" width="24.77734375" customWidth="1"/>
+    <col min="11" max="11" width="23.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CNN1 modified slightly, and minor paths things.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FB2296-0C71-4163-907A-7B6AF6D6C44A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D08EDF-B9A7-4B87-A483-9CB7C05C1950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="171">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -391,9 +391,6 @@
     <t>I think it can be impoved</t>
   </si>
   <si>
-    <t>best among 2</t>
-  </si>
-  <si>
     <t>Best among 5</t>
   </si>
   <si>
@@ -421,9 +418,6 @@
     <t>model_cnn6_4.h5py</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
     <t xml:space="preserve">425505 Bus error               (core dumped) </t>
   </si>
   <si>
@@ -476,6 +470,96 @@
   </si>
   <si>
     <t>Best out of 5, saved</t>
+  </si>
+  <si>
+    <t>Best among 5. Continue training</t>
+  </si>
+  <si>
+    <t>case6_4cont</t>
+  </si>
+  <si>
+    <t>4cont</t>
+  </si>
+  <si>
+    <t>so so, no much improvements from cont</t>
+  </si>
+  <si>
+    <t>not much improvement, but stable</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>3 days runtime</t>
+  </si>
+  <si>
+    <t>not good, overfitting</t>
+  </si>
+  <si>
+    <t>best among 4, bit  not better thatn 16000 images runs</t>
+  </si>
+  <si>
+    <t>good! But not the best I guess</t>
+  </si>
+  <si>
+    <t>case4_2cont</t>
+  </si>
+  <si>
+    <t>case4_20</t>
+  </si>
+  <si>
+    <t>case4_21</t>
+  </si>
+  <si>
+    <t>case4_22</t>
+  </si>
+  <si>
+    <t>case4_23</t>
+  </si>
+  <si>
+    <t>case4_24</t>
+  </si>
+  <si>
+    <t>case4_25</t>
+  </si>
+  <si>
+    <t>modified CNN1 a bit</t>
+  </si>
+  <si>
+    <t>case1_20</t>
+  </si>
+  <si>
+    <t>case1_21</t>
+  </si>
+  <si>
+    <t>case1_22</t>
+  </si>
+  <si>
+    <t>case1_23</t>
+  </si>
+  <si>
+    <t>case1_24</t>
+  </si>
+  <si>
+    <t>case1_25</t>
+  </si>
+  <si>
+    <t>case1_11</t>
+  </si>
+  <si>
+    <t>case1_12</t>
+  </si>
+  <si>
+    <t>case1_13</t>
+  </si>
+  <si>
+    <t>case1_14</t>
+  </si>
+  <si>
+    <t>case1_15</t>
+  </si>
+  <si>
+    <t>case1_16</t>
   </si>
 </sst>
 </file>
@@ -886,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R70"/>
+  <dimension ref="B3:R74"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,7 +1160,7 @@
         <v>38</v>
       </c>
       <c r="I13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J13" s="10"/>
     </row>
@@ -1098,7 +1182,7 @@
         <v>38</v>
       </c>
       <c r="I14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>40</v>
@@ -1122,7 +1206,7 @@
         <v>38</v>
       </c>
       <c r="I15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J15" s="9"/>
     </row>
@@ -1144,46 +1228,65 @@
         <v>38</v>
       </c>
       <c r="I16" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="K16" t="s">
         <v>122</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="K16" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17">
-        <v>811206</v>
+        <v>811742</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
       </c>
-      <c r="E17" s="1">
-        <v>5</v>
+      <c r="E17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J17" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>811206</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G18" s="13"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G20" s="13"/>
-      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="G21" s="13"/>
@@ -1210,7 +1313,7 @@
       <c r="Q22" s="21"/>
       <c r="R22" s="21"/>
     </row>
-    <row r="23" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>14</v>
       </c>
@@ -1431,9 +1534,7 @@
       <c r="E35" s="1">
         <v>1</v>
       </c>
-      <c r="G35" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G35" s="13"/>
       <c r="H35" s="1" t="s">
         <v>50</v>
       </c>
@@ -1454,13 +1555,14 @@
       <c r="E36" s="1">
         <v>2</v>
       </c>
-      <c r="G36" s="13" t="s">
-        <v>7</v>
+      <c r="G36" s="13"/>
+      <c r="J36" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37">
-        <v>811159</v>
+        <v>815294</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -1471,16 +1573,16 @@
       <c r="E37" s="1">
         <v>3</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>124</v>
+      <c r="G37" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="I37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38">
-        <v>811160</v>
+        <v>815295</v>
       </c>
       <c r="C38" t="s">
         <v>55</v>
@@ -1491,16 +1593,16 @@
       <c r="E38" s="1">
         <v>4</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>124</v>
+      <c r="G38" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="I38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39">
-        <v>811161</v>
+        <v>815296</v>
       </c>
       <c r="C39" t="s">
         <v>56</v>
@@ -1511,67 +1613,48 @@
       <c r="E39" s="1">
         <v>5</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>124</v>
+      <c r="G39" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="I39" t="s">
-        <v>125</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>815297</v>
+      </c>
+      <c r="C40" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41">
-        <v>811162</v>
-      </c>
-      <c r="C41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" s="1">
-        <v>2</v>
-      </c>
-      <c r="E41" s="1">
-        <v>1</v>
-      </c>
       <c r="G41" s="13"/>
-      <c r="H41" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B42">
-        <v>811163</v>
-      </c>
-      <c r="C42" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" s="1">
-        <v>2</v>
-      </c>
-      <c r="E42" s="1">
-        <v>2</v>
-      </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43">
-        <v>811164</v>
+        <v>811162</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D43" s="1">
         <v>2</v>
       </c>
       <c r="E43" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G43" s="13"/>
       <c r="H43" s="11" t="s">
@@ -1583,16 +1666,16 @@
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44">
-        <v>811165</v>
+        <v>811163</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D44" s="1">
         <v>2</v>
       </c>
       <c r="E44" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="11" t="s">
@@ -1604,16 +1687,16 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45">
-        <v>811166</v>
+        <v>811164</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D45" s="1">
         <v>2</v>
       </c>
       <c r="E45" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G45" s="13"/>
       <c r="H45" s="11" t="s">
@@ -1623,60 +1706,60 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B48">
-        <v>811174</v>
-      </c>
-      <c r="C48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
-      <c r="E48" s="1">
-        <v>1</v>
-      </c>
-      <c r="G48" s="13"/>
-      <c r="H48" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J48" s="6" t="s">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>811165</v>
+      </c>
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1">
+        <v>4</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B49">
-        <v>811175</v>
-      </c>
-      <c r="C49" t="s">
-        <v>66</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>811166</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="1">
         <v>2</v>
       </c>
-      <c r="G49" s="13"/>
-      <c r="H49" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J49" s="6" t="s">
+      <c r="E47" s="1">
+        <v>5</v>
+      </c>
+      <c r="G47" s="13"/>
+      <c r="H47" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50">
-        <v>811176</v>
+        <v>811174</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G50" s="13"/>
       <c r="H50" s="11" t="s">
@@ -1688,37 +1771,37 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51">
-        <v>811177</v>
+        <v>811175</v>
       </c>
       <c r="C51" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
       </c>
       <c r="E51" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G51" s="13"/>
       <c r="H51" s="11" t="s">
         <v>49</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52">
-        <v>811178</v>
+        <v>811176</v>
       </c>
       <c r="C52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
       <c r="E52" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G52" s="13"/>
       <c r="H52" s="11" t="s">
@@ -1728,66 +1811,60 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>811177</v>
+      </c>
+      <c r="C53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1">
+        <v>4</v>
+      </c>
+      <c r="G53" s="13"/>
+      <c r="H53" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54">
-        <v>811212</v>
+        <v>811178</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
       </c>
       <c r="E54" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G54" s="13"/>
       <c r="H54" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I54" t="s">
-        <v>83</v>
-      </c>
       <c r="J54" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B55">
-        <v>811213</v>
-      </c>
-      <c r="C55" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="1">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1">
-        <v>7</v>
-      </c>
-      <c r="G55" s="13"/>
-      <c r="H55" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I55" t="s">
-        <v>83</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56">
-        <v>811214</v>
+        <v>811212</v>
       </c>
       <c r="C56" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
       </c>
       <c r="E56" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G56" s="13"/>
       <c r="H56" s="11" t="s">
@@ -1800,18 +1877,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B57">
-        <v>811215</v>
+        <v>811213</v>
       </c>
       <c r="C57" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
       </c>
       <c r="E57" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G57" s="13"/>
       <c r="H57" s="11" t="s">
@@ -1821,21 +1898,21 @@
         <v>83</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58">
-        <v>811216</v>
+        <v>811214</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
       </c>
       <c r="E58" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G58" s="13"/>
       <c r="H58" s="11" t="s">
@@ -1844,88 +1921,94 @@
       <c r="I58" t="s">
         <v>83</v>
       </c>
-      <c r="J58" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="K58" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J58" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>811215</v>
+      </c>
+      <c r="C59" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+      <c r="E59" s="1">
+        <v>9</v>
+      </c>
+      <c r="G59" s="13"/>
+      <c r="H59" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I59" t="s">
+        <v>83</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60">
-        <v>811217</v>
+        <v>811216</v>
       </c>
       <c r="C60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D60" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G60" s="13"/>
       <c r="H60" s="11" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I60" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B61">
-        <v>811218</v>
-      </c>
-      <c r="C61" t="s">
-        <v>86</v>
-      </c>
-      <c r="D61" s="1">
-        <v>6</v>
-      </c>
-      <c r="E61" s="1">
-        <v>7</v>
-      </c>
-      <c r="G61" s="13"/>
-      <c r="H61" s="11" t="s">
-        <v>38</v>
+        <v>83</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K60" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B62">
-        <v>811219</v>
+        <v>811217</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D62" s="1">
         <v>6</v>
       </c>
       <c r="E62" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G62" s="13"/>
       <c r="H62" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I62" t="s">
-        <v>119</v>
-      </c>
-      <c r="J62" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63">
-        <v>811220</v>
+        <v>811218</v>
       </c>
       <c r="C63" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D63" s="1">
         <v>6</v>
       </c>
       <c r="E63" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G63" s="13"/>
       <c r="H63" s="11" t="s">
@@ -1934,133 +2017,107 @@
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64">
-        <v>811221</v>
+        <v>811219</v>
       </c>
       <c r="C64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D64" s="1">
         <v>6</v>
       </c>
       <c r="E64" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G64" s="13"/>
       <c r="H64" s="11" t="s">
         <v>38</v>
       </c>
+      <c r="I64" t="s">
+        <v>118</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>811220</v>
+      </c>
+      <c r="C65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="1">
+        <v>6</v>
+      </c>
+      <c r="E65" s="1">
+        <v>9</v>
+      </c>
+      <c r="G65" s="13"/>
+      <c r="H65" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
-        <v>14</v>
+      <c r="B66">
+        <v>811221</v>
       </c>
       <c r="C66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D66" s="1">
         <v>6</v>
       </c>
       <c r="E66" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G66" s="13"/>
       <c r="H66" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I66" t="s">
-        <v>91</v>
-      </c>
-      <c r="J66" s="8" t="s">
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="s">
         <v>142</v>
-      </c>
-      <c r="K66" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B67">
-        <v>811228</v>
-      </c>
-      <c r="C67" t="s">
-        <v>92</v>
       </c>
       <c r="D67" s="1">
         <v>6</v>
       </c>
-      <c r="E67" s="1">
-        <v>12</v>
+      <c r="E67" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G67" s="13"/>
       <c r="H67" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I67" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B68">
-        <v>811229</v>
-      </c>
-      <c r="C68" t="s">
-        <v>93</v>
-      </c>
-      <c r="D68" s="1">
-        <v>6</v>
-      </c>
-      <c r="E68" s="1">
-        <v>13</v>
-      </c>
       <c r="G68" s="13"/>
-      <c r="H68" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I68" t="s">
-        <v>91</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69">
-        <v>811233</v>
-      </c>
-      <c r="C69" t="s">
-        <v>94</v>
-      </c>
-      <c r="D69" s="1">
-        <v>6</v>
-      </c>
-      <c r="E69" s="1">
+      <c r="H68" s="11"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
         <v>14</v>
       </c>
-      <c r="G69" s="13"/>
-      <c r="H69" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I69" t="s">
-        <v>91</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B70">
-        <v>811232</v>
-      </c>
       <c r="C70" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D70" s="1">
         <v>6</v>
       </c>
       <c r="E70" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G70" s="13"/>
       <c r="H70" s="11" t="s">
@@ -2069,7 +2126,106 @@
       <c r="I70" t="s">
         <v>91</v>
       </c>
-      <c r="J70" s="6" t="s">
+      <c r="J70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>811228</v>
+      </c>
+      <c r="C71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="1">
+        <v>6</v>
+      </c>
+      <c r="E71" s="1">
+        <v>12</v>
+      </c>
+      <c r="G71" s="13"/>
+      <c r="H71" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I71" t="s">
+        <v>91</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>811229</v>
+      </c>
+      <c r="C72" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="1">
+        <v>6</v>
+      </c>
+      <c r="E72" s="1">
+        <v>13</v>
+      </c>
+      <c r="G72" s="13"/>
+      <c r="H72" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I72" t="s">
+        <v>91</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>811233</v>
+      </c>
+      <c r="C73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73" s="1">
+        <v>6</v>
+      </c>
+      <c r="E73" s="1">
+        <v>14</v>
+      </c>
+      <c r="G73" s="13"/>
+      <c r="H73" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I73" t="s">
+        <v>91</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>811232</v>
+      </c>
+      <c r="C74" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74" s="1">
+        <v>6</v>
+      </c>
+      <c r="E74" s="1">
+        <v>15</v>
+      </c>
+      <c r="G74" s="13"/>
+      <c r="H74" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I74" t="s">
+        <v>91</v>
+      </c>
+      <c r="J74" s="6" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2087,10 +2243,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
-  <dimension ref="B3:K16"/>
+  <dimension ref="B3:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2150,7 +2306,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="1" t="s">
@@ -2160,7 +2316,7 @@
         <v>96</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>97</v>
@@ -2336,9 +2492,7 @@
       <c r="H14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="18" t="s">
-        <v>114</v>
-      </c>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15">
@@ -2356,11 +2510,12 @@
       <c r="F15" t="b">
         <v>0</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G15" s="13"/>
       <c r="H15" s="11" t="s">
         <v>38</v>
+      </c>
+      <c r="J15" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -2379,11 +2534,168 @@
       <c r="F16" t="b">
         <v>0</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G16" s="13"/>
       <c r="H16" s="11" t="s">
         <v>38</v>
+      </c>
+      <c r="J16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>815311</v>
+      </c>
+      <c r="C18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>11</v>
+      </c>
+      <c r="F18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>815312</v>
+      </c>
+      <c r="C19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>815313</v>
+      </c>
+      <c r="C20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>815314</v>
+      </c>
+      <c r="C21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>14</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>815315</v>
+      </c>
+      <c r="C22" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>15</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>815316</v>
+      </c>
+      <c r="C23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>16</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2395,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1723D785-94D7-412E-814C-F8487739E257}">
-  <dimension ref="B2:K23"/>
+  <dimension ref="B2:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2410,7 +2722,7 @@
     <col min="7" max="7" width="12.88671875" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="19.5546875" customWidth="1"/>
-    <col min="10" max="10" width="24.77734375" customWidth="1"/>
+    <col min="10" max="10" width="25.77734375" customWidth="1"/>
     <col min="11" max="11" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2451,7 +2763,7 @@
         <v>811714</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -2477,7 +2789,7 @@
         <v>811715</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -2500,7 +2812,7 @@
         <v>811716</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -2523,7 +2835,7 @@
         <v>811717</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
@@ -2546,7 +2858,7 @@
         <v>811718</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -2569,7 +2881,7 @@
         <v>811719</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
@@ -2592,7 +2904,7 @@
         <v>811720</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -2615,7 +2927,7 @@
         <v>811721</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
@@ -2638,7 +2950,7 @@
         <v>811722</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -2661,7 +2973,7 @@
         <v>811723</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -2677,6 +2989,9 @@
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="J12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
@@ -2690,7 +3005,7 @@
         <v>811725</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D14" s="1">
         <v>6</v>
@@ -2701,8 +3016,9 @@
       <c r="F14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>7</v>
+      <c r="G14" s="13"/>
+      <c r="J14" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -2710,7 +3026,7 @@
         <v>811726</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -2721,16 +3037,14 @@
       <c r="F15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>811727</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D16" s="1">
         <v>6</v>
@@ -2741,16 +3055,17 @@
       <c r="F16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G16" s="13"/>
+      <c r="J16" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>811728</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
@@ -2761,16 +3076,20 @@
       <c r="F17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="13"/>
+      <c r="I17" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>811729</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D18" s="1">
         <v>6</v>
@@ -2785,12 +3104,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>811730</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D19" s="1">
         <v>6</v>
@@ -2805,23 +3124,289 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>815298</v>
+      </c>
+      <c r="C22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4</v>
+      </c>
+      <c r="E22" s="1">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>815299</v>
+      </c>
+      <c r="C23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1">
+        <v>21</v>
+      </c>
+      <c r="F23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>815300</v>
+      </c>
+      <c r="C24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>815302</v>
+      </c>
+      <c r="C25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="1">
+        <v>4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>23</v>
+      </c>
+      <c r="F25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>815303</v>
+      </c>
+      <c r="C26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1">
+        <v>24</v>
+      </c>
+      <c r="F26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>815304</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1">
+        <v>25</v>
+      </c>
+      <c r="F27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>815305</v>
+      </c>
+      <c r="C30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>20</v>
+      </c>
+      <c r="F30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>815306</v>
+      </c>
+      <c r="C31" t="s">
+        <v>160</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>21</v>
+      </c>
+      <c r="F31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>815307</v>
+      </c>
+      <c r="C32" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>22</v>
+      </c>
+      <c r="F32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>815308</v>
+      </c>
+      <c r="C33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>23</v>
+      </c>
+      <c r="F33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>815309</v>
+      </c>
+      <c r="C34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>24</v>
+      </c>
+      <c r="F34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>815310</v>
+      </c>
+      <c r="C35" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>25</v>
+      </c>
+      <c r="F35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" t="s">
+        <v>158</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
- Started implementing mixed input Keras model. Now, need to organize data (300 images).
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D08EDF-B9A7-4B87-A483-9CB7C05C1950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C043882B-6E95-492A-9AC0-3890E4569331}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16000 data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="172">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -418,9 +418,6 @@
     <t>model_cnn6_4.h5py</t>
   </si>
   <si>
-    <t xml:space="preserve">425505 Bus error               (core dumped) </t>
-  </si>
-  <si>
     <t>case2_20</t>
   </si>
   <si>
@@ -560,6 +557,12 @@
   </si>
   <si>
     <t>case1_16</t>
+  </si>
+  <si>
+    <t>node14</t>
+  </si>
+  <si>
+    <t>Need to run</t>
   </si>
 </sst>
 </file>
@@ -635,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,6 +687,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -972,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R74"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1026,17 +1030,17 @@
     <row r="4" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -1231,7 +1235,7 @@
         <v>121</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K16" t="s">
         <v>122</v>
@@ -1242,13 +1246,13 @@
         <v>811742</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>7</v>
@@ -1261,7 +1265,7 @@
         <v>121</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
@@ -1293,25 +1297,25 @@
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
@@ -1557,12 +1561,12 @@
       </c>
       <c r="G36" s="13"/>
       <c r="J36" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37">
-        <v>815294</v>
+      <c r="B37" s="20">
+        <v>816519</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -1576,13 +1580,10 @@
       <c r="G37" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I37" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38">
-        <v>815295</v>
+      <c r="B38" s="20">
+        <v>816520</v>
       </c>
       <c r="C38" t="s">
         <v>55</v>
@@ -1596,13 +1597,10 @@
       <c r="G38" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I38" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39">
-        <v>815296</v>
+      <c r="B39" s="20">
+        <v>816522</v>
       </c>
       <c r="C39" t="s">
         <v>56</v>
@@ -1616,16 +1614,13 @@
       <c r="G39" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I39" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40">
-        <v>815297</v>
+      <c r="B40" s="20">
+        <v>816523</v>
       </c>
       <c r="C40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D40" s="1">
         <v>4</v>
@@ -2080,13 +2075,13 @@
         <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D67" s="1">
         <v>6</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>7</v>
@@ -2099,7 +2094,7 @@
         <v>121</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.3">
@@ -2127,7 +2122,7 @@
         <v>91</v>
       </c>
       <c r="J70" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K70" t="s">
         <v>99</v>
@@ -2245,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
   <dimension ref="B3:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2254,6 +2249,7 @@
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="43.109375" customWidth="1"/>
     <col min="10" max="10" width="24.21875" customWidth="1"/>
@@ -2515,7 +2511,7 @@
         <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -2539,15 +2535,13 @@
         <v>38</v>
       </c>
       <c r="J16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>815311</v>
-      </c>
+      <c r="B18" s="20"/>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -2559,21 +2553,19 @@
         <v>1</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H18" t="s">
         <v>50</v>
       </c>
       <c r="I18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>815312</v>
-      </c>
+      <c r="B19" s="20"/>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -2585,21 +2577,19 @@
         <v>1</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H19" t="s">
         <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>815313</v>
-      </c>
+      <c r="B20" s="20"/>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -2611,21 +2601,19 @@
         <v>1</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H20" t="s">
         <v>50</v>
       </c>
       <c r="I20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>815314</v>
-      </c>
+      <c r="B21" s="20"/>
       <c r="C21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -2637,21 +2625,19 @@
         <v>0</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H21" t="s">
         <v>50</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>815315</v>
-      </c>
+      <c r="B22" s="20"/>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -2663,21 +2649,19 @@
         <v>0</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H22" t="s">
         <v>50</v>
       </c>
       <c r="I22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>815316</v>
-      </c>
+      <c r="B23" s="20"/>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -2689,13 +2673,13 @@
         <v>0</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H23" t="s">
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2707,10 +2691,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1723D785-94D7-412E-814C-F8487739E257}">
-  <dimension ref="B2:K35"/>
+  <dimension ref="A2:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:I30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2759,11 +2743,11 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>811714</v>
+      <c r="B3" s="20">
+        <v>816584</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -2785,11 +2769,9 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>811715</v>
-      </c>
+      <c r="B4" s="20"/>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -2801,18 +2783,16 @@
         <v>1</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>811716</v>
-      </c>
+      <c r="B5" s="20"/>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -2824,18 +2804,16 @@
         <v>1</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>811717</v>
-      </c>
+      <c r="B6" s="20"/>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
@@ -2847,18 +2825,16 @@
         <v>1</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>811718</v>
-      </c>
+      <c r="B7" s="20"/>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -2870,18 +2846,18 @@
         <v>1</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>811719</v>
+      <c r="B8" s="20">
+        <v>816585</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
@@ -2900,11 +2876,9 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>811720</v>
-      </c>
+      <c r="B9" s="20"/>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -2916,18 +2890,16 @@
         <v>0</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>811721</v>
-      </c>
+      <c r="B10" s="20"/>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
@@ -2939,18 +2911,16 @@
         <v>0</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>811722</v>
-      </c>
+      <c r="B11" s="20"/>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -2962,18 +2932,16 @@
         <v>0</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>811723</v>
-      </c>
+      <c r="B12" s="20"/>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -2985,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -3005,7 +2973,7 @@
         <v>811725</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D14" s="1">
         <v>6</v>
@@ -3018,7 +2986,7 @@
       </c>
       <c r="G14" s="13"/>
       <c r="J14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -3026,7 +2994,7 @@
         <v>811726</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -3044,7 +3012,7 @@
         <v>811727</v>
       </c>
       <c r="C16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="1">
         <v>6</v>
@@ -3057,15 +3025,15 @@
       </c>
       <c r="G16" s="13"/>
       <c r="J16" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>811728</v>
       </c>
       <c r="C17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
@@ -3078,18 +3046,18 @@
       </c>
       <c r="G17" s="13"/>
       <c r="I17" t="s">
+        <v>146</v>
+      </c>
+      <c r="J17" t="s">
         <v>147</v>
       </c>
-      <c r="J17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>811729</v>
       </c>
       <c r="C18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" s="1">
         <v>6</v>
@@ -3104,12 +3072,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>811730</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" s="1">
         <v>6</v>
@@ -3124,20 +3092,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>815298</v>
-      </c>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="20"/>
       <c r="C22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
@@ -3149,15 +3115,13 @@
         <v>1</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>815299</v>
-      </c>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="20"/>
       <c r="C23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
@@ -3169,15 +3133,13 @@
         <v>1</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>815300</v>
-      </c>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="20"/>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -3189,15 +3151,13 @@
         <v>1</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>815302</v>
-      </c>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="20"/>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" s="1">
         <v>4</v>
@@ -3209,15 +3169,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>815303</v>
-      </c>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="20"/>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
@@ -3229,15 +3187,13 @@
         <v>0</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <v>815304</v>
-      </c>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="20"/>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D27" s="1">
         <v>4</v>
@@ -3249,15 +3205,18 @@
         <v>0</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30">
-        <v>815305</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="20">
+        <v>816549</v>
       </c>
       <c r="C30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -3275,15 +3234,13 @@
         <v>50</v>
       </c>
       <c r="I30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31">
-        <v>815306</v>
-      </c>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="20"/>
       <c r="C31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -3295,21 +3252,19 @@
         <v>1</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H31" t="s">
         <v>50</v>
       </c>
       <c r="I31" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32">
-        <v>815307</v>
-      </c>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="20"/>
       <c r="C32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -3321,21 +3276,19 @@
         <v>1</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H32" t="s">
         <v>50</v>
       </c>
       <c r="I32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33">
-        <v>815308</v>
-      </c>
+      <c r="B33" s="20"/>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -3347,21 +3300,19 @@
         <v>0</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H33" t="s">
         <v>50</v>
       </c>
       <c r="I33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34">
-        <v>815309</v>
-      </c>
+      <c r="B34" s="20"/>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -3373,21 +3324,19 @@
         <v>0</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H34" t="s">
         <v>50</v>
       </c>
       <c r="I34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35">
-        <v>815310</v>
-      </c>
+      <c r="B35" s="20"/>
       <c r="C35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -3399,13 +3348,13 @@
         <v>0</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="H35" t="s">
         <v>50</v>
       </c>
       <c r="I35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Proceed with data engineering, write scripts to manipulate data
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C043882B-6E95-492A-9AC0-3890E4569331}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3485D6-487F-4732-8C67-50FB48FD8D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16000 data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="173">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -563,6 +563,9 @@
   </si>
   <si>
     <t>Need to run</t>
+  </si>
+  <si>
+    <t>not bad</t>
   </si>
 </sst>
 </file>
@@ -976,7 +979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="G37" sqref="G37:G40"/>
     </sheetView>
   </sheetViews>
@@ -2240,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
   <dimension ref="B3:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2538,8 +2541,10 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="20"/>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
       <c r="C18" t="s">
         <v>164</v>
       </c>
@@ -2552,18 +2557,21 @@
       <c r="F18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>171</v>
-      </c>
+      <c r="G18" s="13"/>
       <c r="H18" t="s">
         <v>50</v>
       </c>
       <c r="I18" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
+      <c r="J18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
       <c r="C19" t="s">
         <v>165</v>
       </c>
@@ -2576,18 +2584,18 @@
       <c r="F19" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G19" s="13" t="s">
-        <v>171</v>
-      </c>
+      <c r="G19" s="13"/>
       <c r="H19" t="s">
         <v>50</v>
       </c>
       <c r="I19" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="20"/>
+      <c r="J19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>166</v>
       </c>
@@ -2610,7 +2618,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="20"/>
       <c r="C21" t="s">
         <v>167</v>
@@ -2634,7 +2642,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="20"/>
       <c r="C22" t="s">
         <v>168</v>
@@ -2658,7 +2666,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="20"/>
       <c r="C23" t="s">
         <v>169</v>

</xml_diff>

<commit_message>
Proceed with data engineering for the 247 images collection, data generation.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3485D6-487F-4732-8C67-50FB48FD8D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928EF125-644D-427D-BF55-406DFDAD3AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="174">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>not bad</t>
+  </si>
+  <si>
+    <t>not too bad, I thinck adding linear at the end helped</t>
   </si>
 </sst>
 </file>
@@ -2244,7 +2247,7 @@
   <dimension ref="B3:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2255,7 +2258,7 @@
     <col min="7" max="7" width="18.21875" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="43.109375" customWidth="1"/>
-    <col min="10" max="10" width="24.21875" customWidth="1"/>
+    <col min="10" max="10" width="29.6640625" customWidth="1"/>
     <col min="11" max="11" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2542,9 +2545,6 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
       <c r="C18" t="s">
         <v>164</v>
       </c>
@@ -2569,9 +2569,6 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
       <c r="C19" t="s">
         <v>165</v>
       </c>
@@ -2618,7 +2615,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="20"/>
       <c r="C21" t="s">
         <v>167</v>
@@ -2632,14 +2629,15 @@
       <c r="F21" t="b">
         <v>0</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>171</v>
-      </c>
+      <c r="G21" s="13"/>
       <c r="H21" t="s">
         <v>50</v>
       </c>
       <c r="I21" t="s">
         <v>157</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added CNN5 as modified CNN1 after Ahmeds suggestion.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928EF125-644D-427D-BF55-406DFDAD3AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A472D0-043E-454A-8158-1DC421749A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="186">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -568,7 +568,43 @@
     <t>not bad</t>
   </si>
   <si>
-    <t>not too bad, I thinck adding linear at the end helped</t>
+    <t>case1_17</t>
+  </si>
+  <si>
+    <t>model_cnn1_15.h5py</t>
+  </si>
+  <si>
+    <t>best among 4</t>
+  </si>
+  <si>
+    <t>not too bad, I thinc adding linear at the end helped</t>
+  </si>
+  <si>
+    <t>model_cnn1_12.h5py</t>
+  </si>
+  <si>
+    <t>case1_18</t>
+  </si>
+  <si>
+    <t>so far best in 2</t>
+  </si>
+  <si>
+    <t>case5_1</t>
+  </si>
+  <si>
+    <t>modified CNN1 as Ahmed suggested</t>
+  </si>
+  <si>
+    <t>Good, best among 3</t>
+  </si>
+  <si>
+    <t>case5_2</t>
+  </si>
+  <si>
+    <t>case5_3</t>
+  </si>
+  <si>
+    <t>saved</t>
   </si>
 </sst>
 </file>
@@ -982,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R74"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="G37" sqref="G37:G40"/>
     </sheetView>
   </sheetViews>
@@ -2244,9 +2280,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
-  <dimension ref="B3:K23"/>
+  <dimension ref="B3:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -2544,7 +2580,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>164</v>
       </c>
@@ -2568,7 +2604,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>165</v>
       </c>
@@ -2589,10 +2625,13 @@
         <v>157</v>
       </c>
       <c r="J19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="K19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>166</v>
       </c>
@@ -2605,9 +2644,7 @@
       <c r="F20" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>171</v>
-      </c>
+      <c r="G20" s="13"/>
       <c r="H20" t="s">
         <v>50</v>
       </c>
@@ -2615,19 +2652,19 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="20"/>
       <c r="C21" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>14</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="F21" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" t="s">
@@ -2636,56 +2673,168 @@
       <c r="I21" t="s">
         <v>157</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="20"/>
-      <c r="C22" t="s">
-        <v>168</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <v>15</v>
-      </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="H22" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="20"/>
       <c r="C23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>171</v>
-      </c>
+      <c r="G23" s="13"/>
       <c r="H23" t="s">
         <v>50</v>
       </c>
       <c r="I23" t="s">
         <v>157</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>15</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" t="s">
+        <v>157</v>
+      </c>
+      <c r="J24" t="s">
+        <v>175</v>
+      </c>
+      <c r="K24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>169</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>16</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>17</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" t="s">
+        <v>181</v>
+      </c>
+      <c r="J29" t="s">
+        <v>182</v>
+      </c>
+      <c r="K29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>184</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1">
+        <v>3</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First implementation of CNN10 => multiple input KEras model fro the stress-permeability relationship
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A472D0-043E-454A-8158-1DC421749A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38638F2-ADF0-47A9-BF0A-72AD715A369C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16000 data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="199">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -448,24 +448,6 @@
     <t>case2_29</t>
   </si>
   <si>
-    <t>6_21</t>
-  </si>
-  <si>
-    <t>6_22</t>
-  </si>
-  <si>
-    <t>6_23</t>
-  </si>
-  <si>
-    <t>6_24</t>
-  </si>
-  <si>
-    <t>6_25</t>
-  </si>
-  <si>
-    <t>6_26</t>
-  </si>
-  <si>
     <t>Best out of 5, saved</t>
   </si>
   <si>
@@ -605,6 +587,63 @@
   </si>
   <si>
     <t>saved</t>
+  </si>
+  <si>
+    <t>so so</t>
+  </si>
+  <si>
+    <t>overfitting, despite losses are good</t>
+  </si>
+  <si>
+    <t>improved by cont a bit, still train loss is -05</t>
+  </si>
+  <si>
+    <t>case6_21</t>
+  </si>
+  <si>
+    <t>case6_22</t>
+  </si>
+  <si>
+    <t>case6_23</t>
+  </si>
+  <si>
+    <t>case6_24</t>
+  </si>
+  <si>
+    <t>case6_25</t>
+  </si>
+  <si>
+    <t>case6_26</t>
+  </si>
+  <si>
+    <t>case5_4</t>
+  </si>
+  <si>
+    <t>so so, trend is ok</t>
+  </si>
+  <si>
+    <t>case5_5</t>
+  </si>
+  <si>
+    <t>valid is not good</t>
+  </si>
+  <si>
+    <t>case5_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">so so, </t>
+  </si>
+  <si>
+    <t>case5_7</t>
+  </si>
+  <si>
+    <t>case5_8</t>
+  </si>
+  <si>
+    <t>case5_9</t>
+  </si>
+  <si>
+    <t>case5_10</t>
   </si>
 </sst>
 </file>
@@ -680,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -730,11 +769,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1016,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R74"/>
+  <dimension ref="B3:R85"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37:G40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,17 +1117,17 @@
     <row r="4" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -1277,7 +1322,7 @@
         <v>121</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="K16" t="s">
         <v>122</v>
@@ -1288,13 +1333,13 @@
         <v>811742</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>7</v>
@@ -1307,7 +1352,7 @@
         <v>121</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
@@ -1334,942 +1379,1104 @@
         <v>77</v>
       </c>
     </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G19" s="13"/>
+      <c r="H19" s="11"/>
+    </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G21" s="13"/>
-      <c r="H21" s="11"/>
+      <c r="B21">
+        <v>816840</v>
+      </c>
+      <c r="C21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>7</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+      <c r="B22">
+        <v>816841</v>
+      </c>
+      <c r="C22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>8</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>816842</v>
+      </c>
+      <c r="C23" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="1">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>9</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>10</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G25" s="24"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G26" s="24"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G27" s="13"/>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>14</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C29" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D29" s="1">
         <v>4</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J29" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="30" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>14</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="11" t="s">
+      <c r="G30" s="1"/>
+      <c r="H30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="I30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J30" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>14</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C31" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="11" t="s">
+      <c r="G31" s="1"/>
+      <c r="H31" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J25" s="6" t="s">
+      <c r="J31" s="6" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1">
-        <v>11</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" t="s">
-        <v>48</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" t="s">
-        <v>65</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G28" s="1"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D32" s="1">
-        <v>3</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>28</v>
+      <c r="H32" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I32" t="s">
+        <v>48</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I33" t="s">
+        <v>65</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G34" s="1"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>70</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D39" s="1">
         <v>3</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="J39" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="12">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="12">
         <v>811157</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C41" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D41" s="1">
         <v>4</v>
       </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="1" t="s">
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B42">
         <v>811158</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C42" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D42" s="1">
         <v>4</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E42" s="1">
         <v>2</v>
       </c>
-      <c r="G36" s="13"/>
-      <c r="J36" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="20">
+      <c r="G42" s="13"/>
+      <c r="J42" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="20">
         <v>816519</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C43" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D43" s="1">
         <v>4</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E43" s="1">
         <v>3</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G43" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="20">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="20">
         <v>816520</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C44" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D44" s="1">
         <v>4</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E44" s="1">
         <v>4</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="G44" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="20">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="20">
         <v>816522</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C45" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D45" s="1">
         <v>4</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E45" s="1">
         <v>5</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="G45" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="20">
+    <row r="46" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B46" s="20">
         <v>816523</v>
       </c>
-      <c r="C40" t="s">
-        <v>150</v>
-      </c>
-      <c r="D40" s="1">
+      <c r="C46" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" s="1">
         <v>4</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E46" s="1">
         <v>2</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G41" s="13"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B43">
+      <c r="G46" s="13"/>
+      <c r="J46" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G47" s="13"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49">
         <v>811162</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C49" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D49" s="1">
         <v>2</v>
       </c>
-      <c r="E43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="13"/>
-      <c r="H43" s="11" t="s">
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="13"/>
+      <c r="H49" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J43" s="6" t="s">
+      <c r="J49" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B44">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50">
         <v>811163</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C50" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D50" s="1">
         <v>2</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E50" s="1">
         <v>2</v>
-      </c>
-      <c r="G44" s="13"/>
-      <c r="H44" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B45">
-        <v>811164</v>
-      </c>
-      <c r="C45" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="1">
-        <v>2</v>
-      </c>
-      <c r="E45" s="1">
-        <v>3</v>
-      </c>
-      <c r="G45" s="13"/>
-      <c r="H45" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B46">
-        <v>811165</v>
-      </c>
-      <c r="C46" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="1">
-        <v>2</v>
-      </c>
-      <c r="E46" s="1">
-        <v>4</v>
-      </c>
-      <c r="G46" s="13"/>
-      <c r="H46" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47">
-        <v>811166</v>
-      </c>
-      <c r="C47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="1">
-        <v>2</v>
-      </c>
-      <c r="E47" s="1">
-        <v>5</v>
-      </c>
-      <c r="G47" s="13"/>
-      <c r="H47" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B50">
-        <v>811174</v>
-      </c>
-      <c r="C50" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1">
-        <v>1</v>
       </c>
       <c r="G50" s="13"/>
       <c r="H50" s="11" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="J50" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51">
-        <v>811175</v>
+        <v>811164</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D51" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G51" s="13"/>
       <c r="H51" s="11" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="J51" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52">
-        <v>811176</v>
+        <v>811165</v>
       </c>
       <c r="C52" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D52" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E52" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G52" s="13"/>
       <c r="H52" s="11" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="J52" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53">
-        <v>811177</v>
+        <v>811166</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D53" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G53" s="13"/>
       <c r="H53" s="11" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B54">
-        <v>811178</v>
-      </c>
-      <c r="C54" t="s">
-        <v>69</v>
-      </c>
-      <c r="D54" s="1">
-        <v>1</v>
-      </c>
-      <c r="E54" s="1">
-        <v>5</v>
-      </c>
-      <c r="G54" s="13"/>
-      <c r="H54" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J54" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56">
-        <v>811212</v>
+        <v>811174</v>
       </c>
       <c r="C56" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
       </c>
       <c r="E56" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G56" s="13"/>
       <c r="H56" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I56" t="s">
-        <v>83</v>
-      </c>
       <c r="J56" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57">
-        <v>811213</v>
+        <v>811175</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
       </c>
       <c r="E57" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G57" s="13"/>
       <c r="H57" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I57" t="s">
-        <v>83</v>
-      </c>
       <c r="J57" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58">
-        <v>811214</v>
+        <v>811176</v>
       </c>
       <c r="C58" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
       </c>
       <c r="E58" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G58" s="13"/>
       <c r="H58" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I58" t="s">
-        <v>83</v>
-      </c>
       <c r="J58" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59">
-        <v>811215</v>
+        <v>811177</v>
       </c>
       <c r="C59" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
       </c>
       <c r="E59" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G59" s="13"/>
       <c r="H59" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I59" t="s">
-        <v>83</v>
-      </c>
       <c r="J59" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60">
-        <v>811216</v>
+        <v>811178</v>
       </c>
       <c r="C60" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
       </c>
       <c r="E60" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G60" s="13"/>
       <c r="H60" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I60" t="s">
-        <v>83</v>
-      </c>
-      <c r="J60" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="K60" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J60" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62">
-        <v>811217</v>
+        <v>811212</v>
       </c>
       <c r="C62" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D62" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E62" s="1">
         <v>6</v>
       </c>
       <c r="G62" s="13"/>
       <c r="H62" s="11" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I62" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63">
-        <v>811218</v>
+        <v>811213</v>
       </c>
       <c r="C63" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D63" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E63" s="1">
         <v>7</v>
       </c>
       <c r="G63" s="13"/>
       <c r="H63" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="I63" t="s">
+        <v>83</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B64">
-        <v>811219</v>
+        <v>811214</v>
       </c>
       <c r="C64" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D64" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E64" s="1">
         <v>8</v>
       </c>
       <c r="G64" s="13"/>
       <c r="H64" s="11" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I64" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65">
-        <v>811220</v>
+        <v>811215</v>
       </c>
       <c r="C65" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D65" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E65" s="1">
         <v>9</v>
       </c>
       <c r="G65" s="13"/>
       <c r="H65" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="I65" t="s">
+        <v>83</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B66">
-        <v>811221</v>
+        <v>811216</v>
       </c>
       <c r="C66" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D66" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E66" s="1">
         <v>10</v>
       </c>
       <c r="G66" s="13"/>
       <c r="H66" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I66" t="s">
+        <v>83</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K66" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>811217</v>
+      </c>
+      <c r="C68" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="1">
+        <v>6</v>
+      </c>
+      <c r="E68" s="1">
+        <v>6</v>
+      </c>
+      <c r="G68" s="13"/>
+      <c r="H68" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
-        <v>14</v>
-      </c>
-      <c r="C67" t="s">
-        <v>141</v>
-      </c>
-      <c r="D67" s="1">
+      <c r="I68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>811218</v>
+      </c>
+      <c r="C69" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="1">
         <v>6</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F67" s="1" t="s">
+      <c r="E69" s="1">
         <v>7</v>
       </c>
-      <c r="G67" s="13"/>
-      <c r="H67" s="11" t="s">
+      <c r="G69" s="13"/>
+      <c r="H69" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I67" t="s">
-        <v>121</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G68" s="13"/>
-      <c r="H68" s="11"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
-        <v>14</v>
+      <c r="B70">
+        <v>811219</v>
       </c>
       <c r="C70" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D70" s="1">
         <v>6</v>
       </c>
       <c r="E70" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G70" s="13"/>
       <c r="H70" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I70" t="s">
-        <v>91</v>
-      </c>
-      <c r="J70" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="K70" t="s">
-        <v>99</v>
+        <v>118</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B71">
-        <v>811228</v>
+        <v>811220</v>
       </c>
       <c r="C71" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D71" s="1">
         <v>6</v>
       </c>
       <c r="E71" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G71" s="13"/>
       <c r="H71" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I71" t="s">
-        <v>91</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B72">
-        <v>811229</v>
+        <v>811221</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D72" s="1">
         <v>6</v>
       </c>
       <c r="E72" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G72" s="13"/>
       <c r="H72" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I72" t="s">
-        <v>91</v>
-      </c>
-      <c r="J72" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="2:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73">
-        <v>811233</v>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>14</v>
       </c>
       <c r="C73" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="D73" s="1">
         <v>6</v>
       </c>
-      <c r="E73" s="1">
-        <v>14</v>
+      <c r="E73" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G73" s="13"/>
       <c r="H73" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I73" t="s">
+        <v>121</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G74" s="13"/>
+      <c r="H74" s="11"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" t="s">
+        <v>90</v>
+      </c>
+      <c r="D76" s="1">
+        <v>6</v>
+      </c>
+      <c r="E76" s="1">
+        <v>11</v>
+      </c>
+      <c r="G76" s="13"/>
+      <c r="H76" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I76" t="s">
         <v>91</v>
       </c>
-      <c r="J73" s="6" t="s">
+      <c r="J76" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="K76" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>811228</v>
+      </c>
+      <c r="C77" t="s">
+        <v>92</v>
+      </c>
+      <c r="D77" s="1">
+        <v>6</v>
+      </c>
+      <c r="E77" s="1">
+        <v>12</v>
+      </c>
+      <c r="G77" s="13"/>
+      <c r="H77" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I77" t="s">
+        <v>91</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>811229</v>
+      </c>
+      <c r="C78" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" s="1">
+        <v>6</v>
+      </c>
+      <c r="E78" s="1">
+        <v>13</v>
+      </c>
+      <c r="G78" s="13"/>
+      <c r="H78" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I78" t="s">
+        <v>91</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>811233</v>
+      </c>
+      <c r="C79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" s="1">
+        <v>6</v>
+      </c>
+      <c r="E79" s="1">
+        <v>14</v>
+      </c>
+      <c r="G79" s="13"/>
+      <c r="H79" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I79" t="s">
+        <v>91</v>
+      </c>
+      <c r="J79" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B74">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B80">
         <v>811232</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C80" t="s">
         <v>95</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D80" s="1">
         <v>6</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E80" s="1">
         <v>15</v>
       </c>
-      <c r="G74" s="13"/>
-      <c r="H74" s="11" t="s">
+      <c r="G80" s="13"/>
+      <c r="H80" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I80" t="s">
         <v>91</v>
       </c>
-      <c r="J74" s="6" t="s">
+      <c r="J80" s="6" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>189</v>
+      </c>
+      <c r="D83" s="1">
+        <v>5</v>
+      </c>
+      <c r="E83" s="1">
+        <v>4</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I83" t="s">
+        <v>175</v>
+      </c>
+      <c r="J83" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>191</v>
+      </c>
+      <c r="D84" s="1">
+        <v>5</v>
+      </c>
+      <c r="E84" s="1">
+        <v>5</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I84" t="s">
+        <v>175</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>193</v>
+      </c>
+      <c r="D85" s="1">
+        <v>5</v>
+      </c>
+      <c r="E85" s="1">
+        <v>6</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I85" t="s">
+        <v>175</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="K28:R28"/>
     <mergeCell ref="B6:J6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2282,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
   <dimension ref="B3:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2553,7 +2760,7 @@
         <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -2577,12 +2784,12 @@
         <v>38</v>
       </c>
       <c r="J16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -2598,15 +2805,15 @@
         <v>50</v>
       </c>
       <c r="I18" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J18" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -2622,18 +2829,18 @@
         <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J19" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K19" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -2649,13 +2856,13 @@
         <v>50</v>
       </c>
       <c r="I20" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="20"/>
       <c r="C21" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -2671,7 +2878,7 @@
         <v>50</v>
       </c>
       <c r="I21" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
@@ -2680,7 +2887,7 @@
     <row r="23" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="20"/>
       <c r="C23" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -2696,15 +2903,15 @@
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -2720,18 +2927,18 @@
         <v>50</v>
       </c>
       <c r="I24" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J24" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K24" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -2747,12 +2954,12 @@
         <v>50</v>
       </c>
       <c r="I25" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -2768,12 +2975,12 @@
         <v>50</v>
       </c>
       <c r="I26" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D29" s="1">
         <v>5</v>
@@ -2788,18 +2995,18 @@
         <v>50</v>
       </c>
       <c r="I29" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="J29" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="K29" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D30" s="1">
         <v>5</v>
@@ -2814,12 +3021,12 @@
         <v>50</v>
       </c>
       <c r="I30" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D31" s="1">
         <v>5</v>
@@ -2834,7 +3041,7 @@
         <v>50</v>
       </c>
       <c r="I31" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2849,7 +3056,7 @@
   <dimension ref="A2:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2913,14 +3120,14 @@
       <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G3" s="13"/>
       <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="16"/>
-      <c r="J3" s="8"/>
+      <c r="J3" s="21" t="s">
+        <v>180</v>
+      </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
@@ -2938,7 +3145,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>32</v>
@@ -2959,7 +3166,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
@@ -2980,7 +3187,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
@@ -3001,7 +3208,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
@@ -3028,6 +3235,9 @@
       </c>
       <c r="H8" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="J8" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
@@ -3045,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>32</v>
@@ -3066,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>32</v>
@@ -3087,7 +3297,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -3108,7 +3318,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -3128,7 +3338,7 @@
         <v>811725</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>183</v>
       </c>
       <c r="D14" s="1">
         <v>6</v>
@@ -3141,7 +3351,7 @@
       </c>
       <c r="G14" s="13"/>
       <c r="J14" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -3149,7 +3359,7 @@
         <v>811726</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -3167,7 +3377,7 @@
         <v>811727</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>185</v>
       </c>
       <c r="D16" s="1">
         <v>6</v>
@@ -3180,7 +3390,7 @@
       </c>
       <c r="G16" s="13"/>
       <c r="J16" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3188,7 +3398,7 @@
         <v>811728</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>186</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
@@ -3201,10 +3411,10 @@
       </c>
       <c r="G17" s="13"/>
       <c r="I17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3212,7 +3422,7 @@
         <v>811729</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>187</v>
       </c>
       <c r="D18" s="1">
         <v>6</v>
@@ -3232,7 +3442,7 @@
         <v>811730</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>188</v>
       </c>
       <c r="D19" s="1">
         <v>6</v>
@@ -3258,7 +3468,7 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" s="20"/>
       <c r="C22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
@@ -3270,13 +3480,13 @@
         <v>1</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" s="20"/>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
@@ -3288,13 +3498,13 @@
         <v>1</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" s="20"/>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -3306,13 +3516,13 @@
         <v>1</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" s="20"/>
       <c r="C25" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D25" s="1">
         <v>4</v>
@@ -3324,13 +3534,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" s="20"/>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
@@ -3342,13 +3552,13 @@
         <v>0</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" s="20"/>
       <c r="C27" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D27" s="1">
         <v>4</v>
@@ -3360,18 +3570,18 @@
         <v>0</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B30" s="20">
         <v>816549</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -3382,20 +3592,21 @@
       <c r="F30" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>50</v>
       </c>
       <c r="I30" t="s">
-        <v>157</v>
+        <v>151</v>
+      </c>
+      <c r="J30" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31" s="20"/>
       <c r="C31" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -3407,19 +3618,19 @@
         <v>1</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H31" t="s">
         <v>50</v>
       </c>
       <c r="I31" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="20"/>
       <c r="C32" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -3431,19 +3642,19 @@
         <v>1</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H32" t="s">
         <v>50</v>
       </c>
       <c r="I32" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="20"/>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -3455,19 +3666,19 @@
         <v>0</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H33" t="s">
         <v>50</v>
       </c>
       <c r="I33" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="20"/>
       <c r="C34" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -3479,19 +3690,19 @@
         <v>0</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H34" t="s">
         <v>50</v>
       </c>
       <c r="I34" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="20"/>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -3503,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H35" t="s">
         <v>50</v>
       </c>
       <c r="I35" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Made first ~7 runs on CNN10. Results are not good. - In this commit modified cnn10. Need to run.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38638F2-ADF0-47A9-BF0A-72AD715A369C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE74F0-A03A-44A8-B89C-87995F9BC788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16000 data" sheetId="1" r:id="rId1"/>
     <sheet name="16000 Bald data" sheetId="2" r:id="rId2"/>
     <sheet name="65000data" sheetId="3" r:id="rId3"/>
+    <sheet name="247 stress-perm" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="207">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -644,6 +645,30 @@
   </si>
   <si>
     <t>case5_10</t>
+  </si>
+  <si>
+    <t>Not too bad, wait for other runs</t>
+  </si>
+  <si>
+    <t>run10_1</t>
+  </si>
+  <si>
+    <t>run10_2</t>
+  </si>
+  <si>
+    <t>recognizeStressPermf</t>
+  </si>
+  <si>
+    <t>Very bad</t>
+  </si>
+  <si>
+    <t>best among group</t>
+  </si>
+  <si>
+    <t>finished run but failed to save</t>
+  </si>
+  <si>
+    <t>modified CNN10</t>
   </si>
 </sst>
 </file>
@@ -719,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -772,14 +797,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1063,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,7 +1103,7 @@
     <col min="4" max="4" width="5.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" customWidth="1"/>
     <col min="9" max="9" width="60.109375" customWidth="1"/>
     <col min="10" max="10" width="34.6640625" style="6" customWidth="1"/>
@@ -1117,17 +1145,17 @@
     <row r="4" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -1396,7 +1424,7 @@
       <c r="E21" s="1">
         <v>7</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="22" t="s">
         <v>7</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -1419,7 +1447,7 @@
       <c r="E22" s="1">
         <v>8</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="22" t="s">
         <v>7</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -1442,14 +1470,18 @@
       <c r="E23" s="1">
         <v>9</v>
       </c>
-      <c r="G23" s="24" t="s">
-        <v>7</v>
-      </c>
+      <c r="G23" s="22"/>
       <c r="H23" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I23" t="s">
         <v>175</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="K23" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
@@ -1462,7 +1494,7 @@
       <c r="E24" s="1">
         <v>10</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G24" s="22" t="s">
         <v>165</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -1473,11 +1505,11 @@
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G25" s="24"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G26" s="24"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
@@ -1485,25 +1517,25 @@
       <c r="H27" s="11"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
@@ -2489,8 +2521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
   <dimension ref="B3:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3056,7 +3088,7 @@
   <dimension ref="A2:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3727,4 +3759,300 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722B4E69-0002-4323-8973-DCE35F9E32A9}">
+  <dimension ref="B2:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" customWidth="1"/>
+    <col min="11" max="11" width="48.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>816849</v>
+      </c>
+      <c r="C3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="16"/>
+      <c r="J3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>816850</v>
+      </c>
+      <c r="C4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="I4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
No major changes in this commit.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE74F0-A03A-44A8-B89C-87995F9BC788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A41547-84A1-4A7B-BF5E-54BB34528A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16000 data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="211">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -669,6 +669,18 @@
   </si>
   <si>
     <t>modified CNN10</t>
+  </si>
+  <si>
+    <t>run10_11</t>
+  </si>
+  <si>
+    <t>run10_12</t>
+  </si>
+  <si>
+    <t>modified CNN11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad </t>
   </si>
 </sst>
 </file>
@@ -3765,8 +3777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722B4E69-0002-4323-8973-DCE35F9E32A9}">
   <dimension ref="B2:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4023,6 +4035,12 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>816853</v>
+      </c>
+      <c r="C14" t="s">
+        <v>207</v>
+      </c>
       <c r="D14" s="1">
         <v>10</v>
       </c>
@@ -4032,14 +4050,40 @@
       <c r="F14" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="G14" s="13"/>
       <c r="I14" t="s">
         <v>206</v>
       </c>
+      <c r="J14" t="s">
+        <v>210</v>
+      </c>
+      <c r="K14" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="B15">
+        <v>816854</v>
+      </c>
+      <c r="C15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="I15" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
@@ -4054,5 +4098,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Modified cnn10 as results were bad. Now, less of Dropout layers
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A41547-84A1-4A7B-BF5E-54BB34528A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7344B5D2-69D1-46D3-B095-B45DC8A49F80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16000 data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="211">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -479,9 +479,6 @@
     <t>best among 4, bit  not better thatn 16000 images runs</t>
   </si>
   <si>
-    <t>good! But not the best I guess</t>
-  </si>
-  <si>
     <t>case4_2cont</t>
   </si>
   <si>
@@ -647,9 +644,6 @@
     <t>case5_10</t>
   </si>
   <si>
-    <t>Not too bad, wait for other runs</t>
-  </si>
-  <si>
     <t>run10_1</t>
   </si>
   <si>
@@ -677,10 +671,16 @@
     <t>run10_12</t>
   </si>
   <si>
-    <t>modified CNN11</t>
-  </si>
-  <si>
     <t xml:space="preserve">bad </t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>modified again CNN10</t>
+  </si>
+  <si>
+    <t>good! But best among group</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R85"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1428,7 +1428,7 @@
         <v>816840</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D21" s="1">
         <v>5</v>
@@ -1436,14 +1436,15 @@
       <c r="E21" s="1">
         <v>7</v>
       </c>
-      <c r="G21" s="22" t="s">
-        <v>7</v>
-      </c>
+      <c r="G21" s="22"/>
       <c r="H21" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I21" t="s">
-        <v>175</v>
+        <v>174</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
@@ -1451,7 +1452,7 @@
         <v>816841</v>
       </c>
       <c r="C22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D22" s="1">
         <v>5</v>
@@ -1459,14 +1460,12 @@
       <c r="E22" s="1">
         <v>8</v>
       </c>
-      <c r="G22" s="22" t="s">
-        <v>7</v>
-      </c>
+      <c r="G22" s="22"/>
       <c r="H22" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
@@ -1474,7 +1473,7 @@
         <v>816842</v>
       </c>
       <c r="C23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" s="1">
         <v>5</v>
@@ -1487,18 +1486,18 @@
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>175</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>199</v>
+        <v>174</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>202</v>
       </c>
       <c r="K23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D24" s="1">
         <v>5</v>
@@ -1507,13 +1506,13 @@
         <v>10</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
@@ -1793,7 +1792,7 @@
       </c>
       <c r="G42" s="13"/>
       <c r="J42" s="8" t="s">
-        <v>143</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
@@ -1809,9 +1808,7 @@
       <c r="E43" s="1">
         <v>3</v>
       </c>
-      <c r="G43" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G43" s="13"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="20">
@@ -1826,9 +1823,7 @@
       <c r="E44" s="1">
         <v>4</v>
       </c>
-      <c r="G44" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G44" s="13"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="20">
@@ -1852,7 +1847,7 @@
         <v>816523</v>
       </c>
       <c r="C46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1">
         <v>4</v>
@@ -1865,7 +1860,7 @@
       </c>
       <c r="G46" s="13"/>
       <c r="J46" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
@@ -2459,7 +2454,7 @@
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D83" s="1">
         <v>5</v>
@@ -2471,15 +2466,15 @@
         <v>50</v>
       </c>
       <c r="I83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J83" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D84" s="1">
         <v>5</v>
@@ -2491,15 +2486,15 @@
         <v>50</v>
       </c>
       <c r="I84" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J84" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="85" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D85" s="1">
         <v>5</v>
@@ -2511,10 +2506,10 @@
         <v>50</v>
       </c>
       <c r="I85" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2534,7 +2529,7 @@
   <dimension ref="B3:K31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2833,7 +2828,7 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -2849,15 +2844,15 @@
         <v>50</v>
       </c>
       <c r="I18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -2873,18 +2868,18 @@
         <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -2900,13 +2895,13 @@
         <v>50</v>
       </c>
       <c r="I20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="20"/>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -2922,7 +2917,7 @@
         <v>50</v>
       </c>
       <c r="I21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
@@ -2931,7 +2926,7 @@
     <row r="23" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="20"/>
       <c r="C23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -2947,15 +2942,15 @@
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -2971,18 +2966,18 @@
         <v>50</v>
       </c>
       <c r="I24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -2998,12 +2993,12 @@
         <v>50</v>
       </c>
       <c r="I25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -3019,12 +3014,12 @@
         <v>50</v>
       </c>
       <c r="I26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="1">
         <v>5</v>
@@ -3039,18 +3034,18 @@
         <v>50</v>
       </c>
       <c r="I29" t="s">
+        <v>174</v>
+      </c>
+      <c r="J29" t="s">
         <v>175</v>
       </c>
-      <c r="J29" t="s">
-        <v>176</v>
-      </c>
       <c r="K29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D30" s="1">
         <v>5</v>
@@ -3065,12 +3060,12 @@
         <v>50</v>
       </c>
       <c r="I30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D31" s="1">
         <v>5</v>
@@ -3085,7 +3080,7 @@
         <v>50</v>
       </c>
       <c r="I31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3100,7 +3095,7 @@
   <dimension ref="A2:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3170,7 +3165,7 @@
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -3189,7 +3184,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>32</v>
@@ -3210,7 +3205,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
@@ -3231,7 +3226,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
@@ -3252,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
@@ -3281,7 +3276,7 @@
         <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
@@ -3299,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>32</v>
@@ -3320,7 +3315,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>32</v>
@@ -3341,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -3362,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -3382,7 +3377,7 @@
         <v>811725</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D14" s="1">
         <v>6</v>
@@ -3403,7 +3398,7 @@
         <v>811726</v>
       </c>
       <c r="C15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -3421,7 +3416,7 @@
         <v>811727</v>
       </c>
       <c r="C16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D16" s="1">
         <v>6</v>
@@ -3442,7 +3437,7 @@
         <v>811728</v>
       </c>
       <c r="C17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
@@ -3466,7 +3461,7 @@
         <v>811729</v>
       </c>
       <c r="C18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D18" s="1">
         <v>6</v>
@@ -3486,7 +3481,7 @@
         <v>811730</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D19" s="1">
         <v>6</v>
@@ -3512,7 +3507,7 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" s="20"/>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
@@ -3524,13 +3519,13 @@
         <v>1</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" s="20"/>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
@@ -3542,13 +3537,13 @@
         <v>1</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" s="20"/>
       <c r="C24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -3560,13 +3555,13 @@
         <v>1</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" s="20"/>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D25" s="1">
         <v>4</v>
@@ -3578,13 +3573,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" s="20"/>
       <c r="C26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
@@ -3596,13 +3591,13 @@
         <v>0</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" s="20"/>
       <c r="C27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D27" s="1">
         <v>4</v>
@@ -3614,18 +3609,18 @@
         <v>0</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B30" s="20">
         <v>816549</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -3641,16 +3636,16 @@
         <v>50</v>
       </c>
       <c r="I30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31" s="20"/>
       <c r="C31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -3662,19 +3657,19 @@
         <v>1</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H31" t="s">
         <v>50</v>
       </c>
       <c r="I31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="20"/>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -3686,19 +3681,19 @@
         <v>1</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H32" t="s">
         <v>50</v>
       </c>
       <c r="I32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="20"/>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -3710,19 +3705,19 @@
         <v>0</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H33" t="s">
         <v>50</v>
       </c>
       <c r="I33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="20"/>
       <c r="C34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -3734,19 +3729,19 @@
         <v>0</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H34" t="s">
         <v>50</v>
       </c>
       <c r="I34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="20"/>
       <c r="C35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -3758,13 +3753,13 @@
         <v>0</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H35" t="s">
         <v>50</v>
       </c>
       <c r="I35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3777,8 +3772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722B4E69-0002-4323-8973-DCE35F9E32A9}">
   <dimension ref="B2:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3829,7 +3824,7 @@
         <v>816849</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
@@ -3844,7 +3839,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="16"/>
       <c r="J3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -3853,7 +3848,7 @@
         <v>816850</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D4" s="1">
         <v>10</v>
@@ -3866,7 +3861,7 @@
       </c>
       <c r="G4" s="13"/>
       <c r="I4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
@@ -3874,7 +3869,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D5" s="1">
         <v>10</v>
@@ -3886,7 +3881,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
@@ -3894,7 +3889,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D6" s="1">
         <v>10</v>
@@ -3906,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -3914,7 +3909,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D7" s="1">
         <v>10</v>
@@ -3926,7 +3921,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
@@ -3934,7 +3929,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D8" s="1">
         <v>10</v>
@@ -3946,7 +3941,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
@@ -3954,7 +3949,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D9" s="1">
         <v>10</v>
@@ -3966,7 +3961,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
@@ -3974,7 +3969,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D10" s="1">
         <v>10</v>
@@ -3986,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
@@ -3994,7 +3989,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D11" s="1">
         <v>10</v>
@@ -4006,7 +4001,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
@@ -4014,7 +4009,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D12" s="1">
         <v>10</v>
@@ -4026,7 +4021,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
@@ -4035,11 +4030,8 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>816853</v>
-      </c>
       <c r="C14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D14" s="1">
         <v>10</v>
@@ -4052,21 +4044,18 @@
       </c>
       <c r="G14" s="13"/>
       <c r="I14" t="s">
+        <v>204</v>
+      </c>
+      <c r="J14" t="s">
+        <v>207</v>
+      </c>
+      <c r="K14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>206</v>
-      </c>
-      <c r="J14" t="s">
-        <v>210</v>
-      </c>
-      <c r="K14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>816854</v>
-      </c>
-      <c r="C15" t="s">
-        <v>208</v>
       </c>
       <c r="D15" s="1">
         <v>10</v>
@@ -4079,16 +4068,34 @@
       </c>
       <c r="G15" s="13"/>
       <c r="I15" t="s">
+        <v>204</v>
+      </c>
+      <c r="J15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="1">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="I16" t="s">
         <v>209</v>
       </c>
-      <c r="J15" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>

</xml_diff>

<commit_message>
Tried to split differently stress-permf => no effect.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7344B5D2-69D1-46D3-B095-B45DC8A49F80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74882FC3-5AF2-4767-AECD-820C2CA094CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="213">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -674,13 +674,19 @@
     <t xml:space="preserve">bad </t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>modified again CNN10</t>
-  </si>
-  <si>
     <t>good! But best among group</t>
+  </si>
+  <si>
+    <t>better, but validation is problem</t>
+  </si>
+  <si>
+    <t>modified again CNN10, and more changes</t>
+  </si>
+  <si>
+    <t>also  used manual train/valid splitting</t>
+  </si>
+  <si>
+    <t>same as above</t>
   </si>
 </sst>
 </file>
@@ -1792,7 +1798,7 @@
       </c>
       <c r="G42" s="13"/>
       <c r="J42" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
@@ -3770,20 +3776,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722B4E69-0002-4323-8973-DCE35F9E32A9}">
-  <dimension ref="B2:K17"/>
+  <dimension ref="B2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="35.77734375" customWidth="1"/>
+    <col min="10" max="10" width="29.109375" customWidth="1"/>
     <col min="11" max="11" width="48.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4090,17 +4096,208 @@
       <c r="F16" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>208</v>
-      </c>
+      <c r="G16" s="13"/>
       <c r="I16" t="s">
+        <v>210</v>
+      </c>
+      <c r="J16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" s="1">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="I17" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" s="1">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="I18" t="s">
+        <v>210</v>
+      </c>
+      <c r="J18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="1">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="I19" t="s">
+        <v>210</v>
+      </c>
+      <c r="J19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" s="1">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="I20" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D21" s="1">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1">
+        <v>18</v>
+      </c>
+      <c r="F21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="I21" t="s">
+        <v>210</v>
+      </c>
+      <c r="J21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" s="1">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="I23" t="s">
+        <v>211</v>
+      </c>
+      <c r="J23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1">
+        <v>21</v>
+      </c>
+      <c r="F24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="I24" t="s">
+        <v>211</v>
+      </c>
+      <c r="J24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" s="1">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="I25" t="s">
+        <v>211</v>
+      </c>
+      <c r="J25" t="s">
+        <v>212</v>
+      </c>
+      <c r="K25" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
First successful testing on the stress-permf relationship
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74882FC3-5AF2-4767-AECD-820C2CA094CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B3D086-7F42-4A26-A2DE-F9DE33A4C916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="222">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -687,6 +687,33 @@
   </si>
   <si>
     <t>same as above</t>
+  </si>
+  <si>
+    <t>no mixed cnn, but the stress is embedded to image</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>run6_30</t>
+  </si>
+  <si>
+    <t>run6_31</t>
+  </si>
+  <si>
+    <t>better in the stress-permf</t>
+  </si>
+  <si>
+    <t>running 19 days =&gt; had to stop</t>
+  </si>
+  <si>
+    <t>run6_32</t>
+  </si>
+  <si>
+    <t>run6_33</t>
+  </si>
+  <si>
+    <t>run6_34</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R85"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1844,8 +1871,9 @@
       <c r="E45" s="1">
         <v>5</v>
       </c>
-      <c r="G45" s="13" t="s">
-        <v>7</v>
+      <c r="G45" s="13"/>
+      <c r="J45" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2534,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB1FC17-B3C4-4BB9-838D-F9ECB001E049}">
   <dimension ref="B3:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3100,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1723D785-94D7-412E-814C-F8487739E257}">
   <dimension ref="A2:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3189,7 +3217,7 @@
       <c r="F4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -3210,7 +3238,7 @@
       <c r="F5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -3231,7 +3259,7 @@
       <c r="F6" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -3252,7 +3280,7 @@
       <c r="F7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -3275,9 +3303,7 @@
       <c r="F8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="G8" s="2"/>
       <c r="H8" s="1" t="s">
         <v>32</v>
       </c>
@@ -3299,7 +3325,7 @@
       <c r="F9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -3320,7 +3346,7 @@
       <c r="F10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -3341,7 +3367,7 @@
       <c r="F11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -3362,7 +3388,7 @@
       <c r="F12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -3479,7 +3505,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>7</v>
+        <v>164</v>
+      </c>
+      <c r="J18" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3499,7 +3528,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>7</v>
+        <v>164</v>
+      </c>
+      <c r="J19" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3524,7 +3556,7 @@
       <c r="F22" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3542,7 +3574,7 @@
       <c r="F23" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3560,7 +3592,7 @@
       <c r="F24" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3578,7 +3610,7 @@
       <c r="F25" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3596,7 +3628,7 @@
       <c r="F26" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3614,9 +3646,15 @@
       <c r="F27" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="2" t="s">
         <v>164</v>
       </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -3637,7 +3675,7 @@
       <c r="F30" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G30" s="13"/>
+      <c r="G30" s="2"/>
       <c r="H30" t="s">
         <v>50</v>
       </c>
@@ -3662,7 +3700,7 @@
       <c r="F31" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H31" t="s">
@@ -3686,7 +3724,7 @@
       <c r="F32" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H32" t="s">
@@ -3710,7 +3748,7 @@
       <c r="F33" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G33" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H33" t="s">
@@ -3734,7 +3772,7 @@
       <c r="F34" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H34" t="s">
@@ -3758,7 +3796,7 @@
       <c r="F35" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="2" t="s">
         <v>164</v>
       </c>
       <c r="H35" t="s">
@@ -3776,10 +3814,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722B4E69-0002-4323-8973-DCE35F9E32A9}">
-  <dimension ref="B2:K25"/>
+  <dimension ref="B2:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3788,7 +3826,7 @@
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="35.77734375" customWidth="1"/>
+    <col min="9" max="9" width="41.88671875" customWidth="1"/>
     <col min="10" max="10" width="29.109375" customWidth="1"/>
     <col min="11" max="11" width="48.77734375" customWidth="1"/>
   </cols>
@@ -4299,6 +4337,148 @@
         <v>178</v>
       </c>
     </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" s="1">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="I28" t="s">
+        <v>213</v>
+      </c>
+      <c r="J28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>816930</v>
+      </c>
+      <c r="C29" t="s">
+        <v>215</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1">
+        <v>30</v>
+      </c>
+      <c r="F29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="I29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>816931</v>
+      </c>
+      <c r="C30" t="s">
+        <v>216</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1">
+        <v>31</v>
+      </c>
+      <c r="F30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="I30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" s="1">
+        <v>6</v>
+      </c>
+      <c r="E31" s="1">
+        <v>32</v>
+      </c>
+      <c r="F31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="I31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>220</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6</v>
+      </c>
+      <c r="E32" s="1">
+        <v>33</v>
+      </c>
+      <c r="F32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="I32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" s="1">
+        <v>6</v>
+      </c>
+      <c r="E33" s="1">
+        <v>34</v>
+      </c>
+      <c r="F33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="I33" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Improved figures handling and created a separate functions collector for the plots.
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B3D086-7F42-4A26-A2DE-F9DE33A4C916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E29179-670F-45F2-95A3-00D355C8915D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16000 data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="223">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -692,9 +692,6 @@
     <t>no mixed cnn, but the stress is embedded to image</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>run6_30</t>
   </si>
   <si>
@@ -714,6 +711,12 @@
   </si>
   <si>
     <t>run6_34</t>
+  </si>
+  <si>
+    <t>not too bad for beginning</t>
+  </si>
+  <si>
+    <t>saved in selected_models1</t>
   </si>
 </sst>
 </file>
@@ -3508,7 +3511,7 @@
         <v>164</v>
       </c>
       <c r="J18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3531,7 +3534,7 @@
         <v>164</v>
       </c>
       <c r="J19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3816,8 +3819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722B4E69-0002-4323-8973-DCE35F9E32A9}">
   <dimension ref="B2:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4364,10 +4367,10 @@
         <v>213</v>
       </c>
       <c r="J28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K28" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
@@ -4375,7 +4378,7 @@
         <v>816930</v>
       </c>
       <c r="C29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D29" s="1">
         <v>6</v>
@@ -4386,11 +4389,15 @@
       <c r="F29" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>214</v>
-      </c>
+      <c r="G29" s="13"/>
       <c r="I29" t="s">
         <v>213</v>
+      </c>
+      <c r="J29" t="s">
+        <v>221</v>
+      </c>
+      <c r="K29" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
@@ -4398,7 +4405,7 @@
         <v>816931</v>
       </c>
       <c r="C30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D30" s="1">
         <v>6</v>
@@ -4409,11 +4416,15 @@
       <c r="F30" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>214</v>
-      </c>
+      <c r="G30" s="13"/>
       <c r="I30" t="s">
         <v>213</v>
+      </c>
+      <c r="J30" t="s">
+        <v>221</v>
+      </c>
+      <c r="K30" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
@@ -4421,7 +4432,7 @@
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D31" s="1">
         <v>6</v>
@@ -4432,16 +4443,20 @@
       <c r="F31" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G31" s="13" t="s">
-        <v>214</v>
-      </c>
+      <c r="G31" s="13"/>
       <c r="I31" t="s">
         <v>213</v>
       </c>
+      <c r="J31" t="s">
+        <v>221</v>
+      </c>
+      <c r="K31" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D32" s="1">
         <v>6</v>
@@ -4452,16 +4467,20 @@
       <c r="F32" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G32" s="13" t="s">
-        <v>214</v>
-      </c>
+      <c r="G32" s="13"/>
       <c r="I32" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>221</v>
+      </c>
+      <c r="K32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D33" s="1">
         <v>6</v>
@@ -4472,11 +4491,12 @@
       <c r="F33" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G33" s="13" t="s">
-        <v>214</v>
-      </c>
+      <c r="G33" s="13"/>
       <c r="I33" t="s">
         <v>213</v>
+      </c>
+      <c r="J33" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added CNN11  After Ahmed => need to asl him
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E29179-670F-45F2-95A3-00D355C8915D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96062EA-152D-42FE-9E46-9CC24E12154B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16000 data" sheetId="1" r:id="rId1"/>
@@ -3131,7 +3131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1723D785-94D7-412E-814C-F8487739E257}">
   <dimension ref="A2:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -3819,7 +3819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722B4E69-0002-4323-8973-DCE35F9E32A9}">
   <dimension ref="B2:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected bug related to initialization of losses and figures. Deleted cnn10 => as cnn11 is way better!
</commit_message>
<xml_diff>
--- a/Running table.xlsx
+++ b/Running table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\expfracML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96062EA-152D-42FE-9E46-9CC24E12154B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FBF9AB-F215-48D6-A996-0A1AAEA6F686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="228">
   <si>
     <t>recognizeStokes5.py</t>
   </si>
@@ -717,6 +717,21 @@
   </si>
   <si>
     <t>saved in selected_models1</t>
+  </si>
+  <si>
+    <t>modified cnn to cnn11 after Ahmed</t>
+  </si>
+  <si>
+    <t>Way better than cnn10!</t>
+  </si>
+  <si>
+    <t>worse than 11_1</t>
+  </si>
+  <si>
+    <t>1cont</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -3817,10 +3832,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722B4E69-0002-4323-8973-DCE35F9E32A9}">
-  <dimension ref="B2:K33"/>
+  <dimension ref="B2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4346,6 +4361,33 @@
       <c r="F26" s="1"/>
       <c r="G26" s="13"/>
     </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" s="1">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="I27" t="s">
+        <v>223</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="K27" t="s">
+        <v>178</v>
+      </c>
+    </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>14</v>
@@ -4354,115 +4396,61 @@
         <v>200</v>
       </c>
       <c r="D28" s="1">
-        <v>5</v>
-      </c>
-      <c r="E28" s="1">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="F28" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G28" s="13"/>
+      <c r="G28" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="I28" t="s">
-        <v>213</v>
-      </c>
-      <c r="J28" t="s">
-        <v>216</v>
-      </c>
-      <c r="K28" t="s">
-        <v>222</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <v>816930</v>
+      <c r="B29" t="s">
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="D29" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G29" s="13"/>
       <c r="I29" t="s">
-        <v>213</v>
-      </c>
-      <c r="J29" t="s">
-        <v>221</v>
-      </c>
-      <c r="K29" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30">
-        <v>816931</v>
-      </c>
-      <c r="C30" t="s">
-        <v>215</v>
-      </c>
-      <c r="D30" s="1">
-        <v>6</v>
-      </c>
-      <c r="E30" s="1">
-        <v>31</v>
-      </c>
-      <c r="F30" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G30" s="13"/>
-      <c r="I30" t="s">
-        <v>213</v>
-      </c>
-      <c r="J30" t="s">
-        <v>221</v>
-      </c>
-      <c r="K30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+        <v>223</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>14</v>
       </c>
-      <c r="C31" t="s">
-        <v>218</v>
-      </c>
-      <c r="D31" s="1">
-        <v>6</v>
-      </c>
-      <c r="E31" s="1">
-        <v>32</v>
-      </c>
-      <c r="F31" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G31" s="13"/>
-      <c r="I31" t="s">
-        <v>213</v>
-      </c>
-      <c r="J31" t="s">
-        <v>221</v>
-      </c>
-      <c r="K31" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="D32" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F32" s="1" t="b">
         <v>0</v>
@@ -4472,21 +4460,24 @@
         <v>213</v>
       </c>
       <c r="J32" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="K32" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>816930</v>
+      </c>
       <c r="C33" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D33" s="1">
         <v>6</v>
       </c>
       <c r="E33" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F33" s="1" t="b">
         <v>0</v>
@@ -4496,6 +4487,108 @@
         <v>213</v>
       </c>
       <c r="J33" t="s">
+        <v>221</v>
+      </c>
+      <c r="K33" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>816931</v>
+      </c>
+      <c r="C34" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6</v>
+      </c>
+      <c r="E34" s="1">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="I34" t="s">
+        <v>213</v>
+      </c>
+      <c r="J34" t="s">
+        <v>221</v>
+      </c>
+      <c r="K34" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" s="1">
+        <v>6</v>
+      </c>
+      <c r="E35" s="1">
+        <v>32</v>
+      </c>
+      <c r="F35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="I35" t="s">
+        <v>213</v>
+      </c>
+      <c r="J35" t="s">
+        <v>221</v>
+      </c>
+      <c r="K35" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>219</v>
+      </c>
+      <c r="D36" s="1">
+        <v>6</v>
+      </c>
+      <c r="E36" s="1">
+        <v>33</v>
+      </c>
+      <c r="F36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="I36" t="s">
+        <v>213</v>
+      </c>
+      <c r="J36" t="s">
+        <v>221</v>
+      </c>
+      <c r="K36" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>220</v>
+      </c>
+      <c r="D37" s="1">
+        <v>6</v>
+      </c>
+      <c r="E37" s="1">
+        <v>34</v>
+      </c>
+      <c r="F37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="I37" t="s">
+        <v>213</v>
+      </c>
+      <c r="J37" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>